<commit_message>
New jpg's added plus feladatok pdf
</commit_message>
<xml_diff>
--- a/Gyerekek.xlsx
+++ b/Gyerekek.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Privat\Informatika\Github\ZitaTuroczi1.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21686616-AE45-46C2-9A46-F15B2B835883}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADEB8DA5-712F-4655-93ED-BC70DE078A51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="885" windowWidth="13455" windowHeight="14865" xr2:uid="{D8DA68CD-37D4-4C3C-BD5C-8E37EBBBD311}"/>
+    <workbookView xWindow="4770" yWindow="870" windowWidth="13455" windowHeight="14865" xr2:uid="{D8DA68CD-37D4-4C3C-BD5C-8E37EBBBD311}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="224">
   <si>
     <t xml:space="preserve">Előképző 
 </t>
@@ -701,6 +701,9 @@
   </si>
   <si>
     <t>Sóvári Dénes</t>
+  </si>
+  <si>
+    <t>Anyák napja</t>
   </si>
 </sst>
 </file>
@@ -1341,8 +1344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9286C3FF-60BE-42C4-89D5-9ACF7C2ACF54}">
   <dimension ref="A2:M95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H90" sqref="H90"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L56" sqref="L56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1505,7 +1508,7 @@
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
       <c r="F8" s="22"/>
-      <c r="G8" s="15"/>
+      <c r="G8" s="22"/>
       <c r="H8" s="15"/>
       <c r="J8" s="13" t="s">
         <v>22</v>
@@ -1549,7 +1552,7 @@
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
-      <c r="G10" s="3"/>
+      <c r="G10" s="22"/>
       <c r="H10" s="3"/>
       <c r="J10" s="13" t="s">
         <v>26</v>
@@ -1572,7 +1575,7 @@
       <c r="D11" s="22"/>
       <c r="E11" s="22"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
+      <c r="G11" s="22"/>
       <c r="H11" s="3"/>
       <c r="J11" s="13" t="s">
         <v>29</v>
@@ -1593,7 +1596,7 @@
       <c r="D12" s="22"/>
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
-      <c r="G12" s="3"/>
+      <c r="G12" s="22"/>
       <c r="H12" s="3"/>
       <c r="J12" s="13" t="s">
         <v>32</v>
@@ -1673,7 +1676,7 @@
       <c r="C17" s="24"/>
       <c r="D17" s="23"/>
       <c r="E17" s="23"/>
-      <c r="F17" s="20"/>
+      <c r="F17" s="23"/>
       <c r="G17" s="20"/>
       <c r="H17" s="20"/>
       <c r="J17" s="13" t="s">
@@ -1695,7 +1698,7 @@
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
       <c r="F18" s="22"/>
-      <c r="G18" s="15"/>
+      <c r="G18" s="22"/>
       <c r="H18" s="15"/>
       <c r="J18" s="13" t="s">
         <v>50</v>
@@ -1762,7 +1765,7 @@
       <c r="D21" s="22"/>
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
-      <c r="G21" s="15"/>
+      <c r="G21" s="22"/>
       <c r="H21" s="15"/>
       <c r="J21" s="13" t="s">
         <v>58</v>
@@ -1783,7 +1786,7 @@
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
-      <c r="G22" s="15"/>
+      <c r="G22" s="22"/>
       <c r="H22" s="15"/>
       <c r="J22" s="13" t="s">
         <v>60</v>
@@ -1867,7 +1870,7 @@
       <c r="D26" s="22"/>
       <c r="E26" s="22"/>
       <c r="F26" s="22"/>
-      <c r="G26" s="3"/>
+      <c r="G26" s="22"/>
       <c r="H26" s="3"/>
       <c r="J26" s="13" t="s">
         <v>68</v>
@@ -1926,7 +1929,7 @@
       <c r="D29" s="22"/>
       <c r="E29" s="3"/>
       <c r="F29" s="22"/>
-      <c r="G29" s="3"/>
+      <c r="G29" s="22"/>
       <c r="H29" s="3"/>
       <c r="J29" s="13" t="s">
         <v>71</v>
@@ -2324,7 +2327,7 @@
       <c r="D50" s="22"/>
       <c r="E50" s="22"/>
       <c r="F50" s="22"/>
-      <c r="G50" s="15"/>
+      <c r="G50" s="22"/>
       <c r="H50" s="15"/>
       <c r="J50" s="13" t="s">
         <v>116</v>
@@ -2344,7 +2347,7 @@
       <c r="C51" s="21"/>
       <c r="D51" s="22"/>
       <c r="E51" s="15"/>
-      <c r="F51" s="15"/>
+      <c r="F51" s="22"/>
       <c r="G51" s="15"/>
       <c r="H51" s="15"/>
       <c r="J51" s="13" t="s">
@@ -2365,7 +2368,7 @@
       <c r="C52" s="25"/>
       <c r="D52" s="22"/>
       <c r="E52" s="15"/>
-      <c r="F52" s="15"/>
+      <c r="F52" s="22"/>
       <c r="G52" s="15"/>
       <c r="H52" s="15"/>
       <c r="J52" s="13" t="s">
@@ -2467,7 +2470,7 @@
       <c r="E58" s="22"/>
       <c r="F58" s="22"/>
       <c r="G58" s="22"/>
-      <c r="H58" s="15"/>
+      <c r="H58" s="22"/>
       <c r="J58" s="13" t="s">
         <v>135</v>
       </c>
@@ -2574,7 +2577,7 @@
       <c r="E63" s="22"/>
       <c r="F63" s="22"/>
       <c r="G63" s="22"/>
-      <c r="H63" s="15"/>
+      <c r="H63" s="22"/>
       <c r="J63" s="13" t="s">
         <v>66</v>
       </c>
@@ -2595,7 +2598,7 @@
       <c r="E64" s="22"/>
       <c r="F64" s="22"/>
       <c r="G64" s="22"/>
-      <c r="H64" s="15"/>
+      <c r="H64" s="22"/>
       <c r="J64" s="13" t="s">
         <v>146</v>
       </c>
@@ -2616,7 +2619,7 @@
       <c r="E65" s="22"/>
       <c r="F65" s="22"/>
       <c r="G65" s="22"/>
-      <c r="H65" s="15"/>
+      <c r="H65" s="22"/>
       <c r="J65" s="13" t="s">
         <v>148</v>
       </c>
@@ -2733,7 +2736,7 @@
       <c r="C72" s="19"/>
       <c r="D72" s="23"/>
       <c r="E72" s="20"/>
-      <c r="F72" s="20"/>
+      <c r="F72" s="23"/>
       <c r="G72" s="20"/>
       <c r="H72" s="4"/>
       <c r="J72" s="13" t="s">
@@ -2878,7 +2881,7 @@
       <c r="D79" s="22"/>
       <c r="E79" s="3"/>
       <c r="F79" s="22"/>
-      <c r="G79" s="3"/>
+      <c r="G79" s="22"/>
       <c r="H79" s="3"/>
       <c r="J79" s="13" t="s">
         <v>176</v>
@@ -2898,7 +2901,7 @@
       <c r="C80" s="25"/>
       <c r="D80" s="22"/>
       <c r="E80" s="22"/>
-      <c r="F80" s="3"/>
+      <c r="F80" s="22"/>
       <c r="G80" s="22"/>
       <c r="H80" s="3"/>
       <c r="J80" s="13" t="s">
@@ -2983,7 +2986,7 @@
       <c r="D84" s="22"/>
       <c r="E84" s="22"/>
       <c r="F84" s="22"/>
-      <c r="G84" s="3"/>
+      <c r="G84" s="22"/>
       <c r="H84" s="3"/>
       <c r="J84" s="13" t="s">
         <v>186</v>
@@ -3028,7 +3031,9 @@
       <c r="D88" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="E88" s="2"/>
+      <c r="E88" s="2" t="s">
+        <v>223</v>
+      </c>
       <c r="F88" s="2"/>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
@@ -3048,7 +3053,9 @@
       <c r="D89" s="8">
         <v>43942</v>
       </c>
-      <c r="E89" s="8"/>
+      <c r="E89" s="8">
+        <v>43949</v>
+      </c>
       <c r="F89" s="8"/>
       <c r="G89" s="8"/>
       <c r="H89" s="8"/>
@@ -3087,7 +3094,7 @@
       </c>
       <c r="C91" s="25"/>
       <c r="D91" s="22"/>
-      <c r="E91" s="15"/>
+      <c r="E91" s="22"/>
       <c r="F91" s="15"/>
       <c r="G91" s="15"/>
       <c r="H91" s="15"/>
@@ -3129,7 +3136,7 @@
       </c>
       <c r="C93" s="25"/>
       <c r="D93" s="15"/>
-      <c r="E93" s="15"/>
+      <c r="E93" s="22"/>
       <c r="F93" s="15"/>
       <c r="G93" s="15"/>
       <c r="H93" s="15"/>

</xml_diff>

<commit_message>
04_06 new drawings and another try to display tablazat
</commit_message>
<xml_diff>
--- a/Gyerekek.xlsx
+++ b/Gyerekek.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Privat\Informatika\Github\ZitaTuroczi1.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D197B1B-DFFF-476D-9723-883810746984}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB4168FC-04A3-4EC1-9226-C2CA65191B85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4770" yWindow="870" windowWidth="13455" windowHeight="14865" xr2:uid="{D8DA68CD-37D4-4C3C-BD5C-8E37EBBBD311}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{D8DA68CD-37D4-4C3C-BD5C-8E37EBBBD311}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -1344,8 +1344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9286C3FF-60BE-42C4-89D5-9ACF7C2ACF54}">
   <dimension ref="A2:M95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I88" sqref="I88"/>
+    <sheetView tabSelected="1" topLeftCell="A71" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J97" sqref="J97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1677,7 +1677,7 @@
       <c r="D17" s="23"/>
       <c r="E17" s="23"/>
       <c r="F17" s="23"/>
-      <c r="G17" s="20"/>
+      <c r="G17" s="23"/>
       <c r="H17" s="20"/>
       <c r="J17" s="13" t="s">
         <v>48</v>
@@ -2303,9 +2303,9 @@
         <v>104</v>
       </c>
       <c r="C49" s="21"/>
-      <c r="D49" s="15"/>
+      <c r="D49" s="22"/>
       <c r="E49" s="15"/>
-      <c r="F49" s="15"/>
+      <c r="F49" s="22"/>
       <c r="G49" s="15"/>
       <c r="H49" s="15"/>
       <c r="J49" s="13" t="s">
@@ -3135,7 +3135,7 @@
         <v>193</v>
       </c>
       <c r="C93" s="25"/>
-      <c r="D93" s="15"/>
+      <c r="D93" s="22"/>
       <c r="E93" s="22"/>
       <c r="F93" s="15"/>
       <c r="G93" s="15"/>
@@ -3159,7 +3159,7 @@
       </c>
       <c r="C94" s="25"/>
       <c r="D94" s="22"/>
-      <c r="E94" s="15"/>
+      <c r="E94" s="22"/>
       <c r="F94" s="15"/>
       <c r="G94" s="15"/>
       <c r="H94" s="15"/>
@@ -3179,7 +3179,7 @@
       </c>
       <c r="C95" s="25"/>
       <c r="D95" s="22"/>
-      <c r="E95" s="15"/>
+      <c r="E95" s="22"/>
       <c r="F95" s="15"/>
       <c r="G95" s="15"/>
       <c r="H95" s="15"/>

</xml_diff>

<commit_message>
04.11_new files from 04.07-08
</commit_message>
<xml_diff>
--- a/Gyerekek.xlsx
+++ b/Gyerekek.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Privat\Informatika\Github\ZitaTuroczi1.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB4168FC-04A3-4EC1-9226-C2CA65191B85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC273282-A490-43F5-BE10-EB29EFBF8488}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{D8DA68CD-37D4-4C3C-BD5C-8E37EBBBD311}"/>
+    <workbookView xWindow="12735" yWindow="330" windowWidth="13455" windowHeight="14865" xr2:uid="{D8DA68CD-37D4-4C3C-BD5C-8E37EBBBD311}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="225">
   <si>
     <t xml:space="preserve">Előképző 
 </t>
@@ -704,6 +704,9 @@
   </si>
   <si>
     <t>Anyák napja</t>
+  </si>
+  <si>
+    <t>Pillangó hajtogatása</t>
   </si>
 </sst>
 </file>
@@ -968,7 +971,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
@@ -1027,6 +1030,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hivatkozás" xfId="1" builtinId="8"/>
@@ -1342,10 +1358,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9286C3FF-60BE-42C4-89D5-9ACF7C2ACF54}">
-  <dimension ref="A2:M95"/>
+  <dimension ref="A2:N95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J97" sqref="J97"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L63" sqref="L63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1353,13 +1369,14 @@
     <col min="1" max="1" width="4.42578125" customWidth="1"/>
     <col min="2" max="2" width="26.7109375" style="31" bestFit="1" customWidth="1"/>
     <col min="3" max="8" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" customWidth="1"/>
-    <col min="12" max="12" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.7109375" style="31" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" customWidth="1"/>
+    <col min="13" max="13" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" s="1" customFormat="1" ht="106.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="1" customFormat="1" ht="106.5" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
@@ -1384,8 +1401,9 @@
       <c r="H2" s="2" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" s="1" customFormat="1" ht="42" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I2" s="33"/>
+    </row>
+    <row r="3" spans="1:13" s="1" customFormat="1" ht="42" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
       <c r="B3" s="28">
         <v>2020</v>
@@ -1408,8 +1426,9 @@
       <c r="H3" s="8">
         <v>43950</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I3" s="34"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>1</v>
       </c>
@@ -1422,15 +1441,16 @@
       <c r="F4" s="23"/>
       <c r="G4" s="20"/>
       <c r="H4" s="20"/>
-      <c r="J4" s="13" t="s">
+      <c r="I4" s="32"/>
+      <c r="K4" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="13"/>
-      <c r="L4" s="14" t="s">
+      <c r="L4" s="13"/>
+      <c r="M4" s="14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>2</v>
       </c>
@@ -1443,17 +1463,18 @@
       <c r="F5" s="22"/>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
-      <c r="J5" s="13" t="s">
+      <c r="I5" s="32"/>
+      <c r="K5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="K5" s="13" t="s">
+      <c r="L5" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="L5" s="14" t="s">
+      <c r="M5" s="14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>3</v>
       </c>
@@ -1466,17 +1487,18 @@
       <c r="F6" s="22"/>
       <c r="G6" s="22"/>
       <c r="H6" s="15"/>
-      <c r="J6" s="13" t="s">
+      <c r="I6" s="32"/>
+      <c r="K6" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="K6" s="13" t="s">
+      <c r="L6" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="L6" s="14" t="s">
+      <c r="M6" s="14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>4</v>
       </c>
@@ -1489,15 +1511,16 @@
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
-      <c r="J7" s="13" t="s">
+      <c r="I7" s="32"/>
+      <c r="K7" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="K7" s="13"/>
-      <c r="L7" s="14" t="s">
+      <c r="L7" s="13"/>
+      <c r="M7" s="14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>5</v>
       </c>
@@ -1510,15 +1533,16 @@
       <c r="F8" s="22"/>
       <c r="G8" s="22"/>
       <c r="H8" s="15"/>
-      <c r="J8" s="13" t="s">
+      <c r="I8" s="32"/>
+      <c r="K8" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="K8" s="13"/>
-      <c r="L8" s="14" t="s">
+      <c r="L8" s="13"/>
+      <c r="M8" s="14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>6</v>
       </c>
@@ -1531,17 +1555,18 @@
       <c r="F9" s="22"/>
       <c r="G9" s="22"/>
       <c r="H9" s="15"/>
-      <c r="J9" s="13" t="s">
+      <c r="I9" s="32"/>
+      <c r="K9" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="K9" s="13" t="s">
+      <c r="L9" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="L9" s="14" t="s">
+      <c r="M9" s="14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>7</v>
       </c>
@@ -1554,17 +1579,18 @@
       <c r="F10" s="22"/>
       <c r="G10" s="22"/>
       <c r="H10" s="3"/>
-      <c r="J10" s="13" t="s">
+      <c r="I10" s="32"/>
+      <c r="K10" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="K10" s="13" t="s">
+      <c r="L10" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="L10" s="14" t="s">
+      <c r="M10" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>8</v>
       </c>
@@ -1576,16 +1602,17 @@
       <c r="E11" s="22"/>
       <c r="F11" s="3"/>
       <c r="G11" s="22"/>
-      <c r="H11" s="3"/>
-      <c r="J11" s="13" t="s">
+      <c r="H11" s="22"/>
+      <c r="I11" s="32"/>
+      <c r="K11" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="K11" s="13"/>
-      <c r="L11" s="14" t="s">
+      <c r="L11" s="13"/>
+      <c r="M11" s="14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>9</v>
       </c>
@@ -1598,17 +1625,18 @@
       <c r="F12" s="22"/>
       <c r="G12" s="22"/>
       <c r="H12" s="3"/>
-      <c r="J12" s="13" t="s">
+      <c r="I12" s="32"/>
+      <c r="K12" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="K12" s="13" t="s">
+      <c r="L12" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="L12" s="14" t="s">
+      <c r="M12" s="14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="106.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="106.5" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>0</v>
       </c>
@@ -1633,12 +1661,13 @@
       <c r="H15" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="I15" s="1"/>
+      <c r="I15" s="33"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-    </row>
-    <row r="16" spans="1:12" ht="42" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M15" s="1"/>
+    </row>
+    <row r="16" spans="1:13" ht="42" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10"/>
       <c r="B16" s="28">
         <v>2020</v>
@@ -1661,12 +1690,13 @@
       <c r="H16" s="8">
         <v>43950</v>
       </c>
-      <c r="I16" s="1"/>
+      <c r="I16" s="34"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M16" s="1"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <v>1</v>
       </c>
@@ -1679,15 +1709,16 @@
       <c r="F17" s="23"/>
       <c r="G17" s="23"/>
       <c r="H17" s="20"/>
-      <c r="J17" s="13" t="s">
+      <c r="I17" s="32"/>
+      <c r="K17" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="K17" s="13"/>
-      <c r="L17" s="14" t="s">
+      <c r="L17" s="13"/>
+      <c r="M17" s="14" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>2</v>
       </c>
@@ -1700,17 +1731,18 @@
       <c r="F18" s="22"/>
       <c r="G18" s="22"/>
       <c r="H18" s="15"/>
-      <c r="J18" s="13" t="s">
+      <c r="I18" s="32"/>
+      <c r="K18" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="K18" s="13" t="s">
+      <c r="L18" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="L18" s="14" t="s">
+      <c r="M18" s="14" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>3</v>
       </c>
@@ -1723,17 +1755,18 @@
       <c r="F19" s="22"/>
       <c r="G19" s="15"/>
       <c r="H19" s="15"/>
-      <c r="J19" s="13" t="s">
+      <c r="I19" s="32"/>
+      <c r="K19" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="K19" s="13" t="s">
+      <c r="L19" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="L19" s="14" t="s">
+      <c r="M19" s="14" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>4</v>
       </c>
@@ -1746,15 +1779,16 @@
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
-      <c r="J20" s="13" t="s">
+      <c r="I20" s="32"/>
+      <c r="K20" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="K20" s="13"/>
-      <c r="L20" s="14" t="s">
+      <c r="L20" s="13"/>
+      <c r="M20" s="14" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>5</v>
       </c>
@@ -1767,15 +1801,16 @@
       <c r="F21" s="22"/>
       <c r="G21" s="22"/>
       <c r="H21" s="15"/>
-      <c r="J21" s="13" t="s">
+      <c r="I21" s="32"/>
+      <c r="K21" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="K21" s="13"/>
-      <c r="L21" s="14" t="s">
+      <c r="L21" s="13"/>
+      <c r="M21" s="14" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>6</v>
       </c>
@@ -1788,15 +1823,16 @@
       <c r="F22" s="22"/>
       <c r="G22" s="22"/>
       <c r="H22" s="15"/>
-      <c r="J22" s="13" t="s">
+      <c r="I22" s="32"/>
+      <c r="K22" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="K22" s="13"/>
-      <c r="L22" s="14" t="s">
+      <c r="L22" s="13"/>
+      <c r="M22" s="14" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <v>7</v>
       </c>
@@ -1807,17 +1843,18 @@
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
       <c r="F23" s="22"/>
-      <c r="G23" s="15"/>
+      <c r="G23" s="22"/>
       <c r="H23" s="15"/>
-      <c r="J23" s="13" t="s">
+      <c r="I23" s="32"/>
+      <c r="K23" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="K23" s="13"/>
-      <c r="L23" s="14" t="s">
+      <c r="L23" s="13"/>
+      <c r="M23" s="14" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="16">
         <v>8</v>
       </c>
@@ -1830,15 +1867,16 @@
       <c r="F24" s="22"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
-      <c r="J24" s="13" t="s">
+      <c r="I24" s="32"/>
+      <c r="K24" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="K24" s="13"/>
-      <c r="L24" s="14" t="s">
+      <c r="L24" s="13"/>
+      <c r="M24" s="14" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="16">
         <v>9</v>
       </c>
@@ -1851,15 +1889,16 @@
       <c r="F25" s="22"/>
       <c r="G25" s="22"/>
       <c r="H25" s="3"/>
-      <c r="J25" s="13" t="s">
+      <c r="I25" s="32"/>
+      <c r="K25" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="K25" s="13"/>
-      <c r="L25" s="14" t="s">
+      <c r="L25" s="13"/>
+      <c r="M25" s="14" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="17">
         <v>10</v>
       </c>
@@ -1872,13 +1911,14 @@
       <c r="F26" s="22"/>
       <c r="G26" s="22"/>
       <c r="H26" s="3"/>
-      <c r="J26" s="13" t="s">
+      <c r="I26" s="32"/>
+      <c r="K26" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="K26" s="13"/>
-      <c r="L26" s="14"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L26" s="13"/>
+      <c r="M26" s="14"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="17">
         <v>11</v>
       </c>
@@ -1891,17 +1931,18 @@
       <c r="F27" s="22"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
-      <c r="J27" s="13" t="s">
+      <c r="I27" s="32"/>
+      <c r="K27" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="K27" s="13" t="s">
+      <c r="L27" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="L27" s="14" t="s">
+      <c r="M27" s="14" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="17">
         <v>12</v>
       </c>
@@ -1914,11 +1955,12 @@
       <c r="F28" s="22"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
-      <c r="J28" s="13"/>
+      <c r="I28" s="32"/>
       <c r="K28" s="13"/>
-      <c r="L28" s="14"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L28" s="13"/>
+      <c r="M28" s="14"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="17">
         <v>13</v>
       </c>
@@ -1931,15 +1973,16 @@
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
       <c r="H29" s="3"/>
-      <c r="J29" s="13" t="s">
+      <c r="I29" s="32"/>
+      <c r="K29" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="K29" s="13"/>
-      <c r="L29" s="14" t="s">
+      <c r="L29" s="13"/>
+      <c r="M29" s="14" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="106.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="106.5" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>0</v>
       </c>
@@ -1964,12 +2007,13 @@
       <c r="H32" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="I32" s="1"/>
+      <c r="I32" s="33"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
-    </row>
-    <row r="33" spans="1:13" ht="42" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M32" s="1"/>
+    </row>
+    <row r="33" spans="1:14" ht="42" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="10"/>
       <c r="B33" s="28">
         <v>2020</v>
@@ -1992,12 +2036,13 @@
       <c r="H33" s="8">
         <v>43950</v>
       </c>
-      <c r="I33" s="1"/>
+      <c r="I33" s="34"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M33" s="1"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="11">
         <v>1</v>
       </c>
@@ -2010,20 +2055,21 @@
       <c r="F34" s="23"/>
       <c r="G34" s="20"/>
       <c r="H34" s="20"/>
-      <c r="J34" s="13" t="s">
+      <c r="I34" s="32"/>
+      <c r="K34" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="K34" s="13" t="s">
+      <c r="L34" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="L34" s="14" t="s">
+      <c r="M34" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="M34" s="14" t="s">
+      <c r="N34" s="14" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <v>2</v>
       </c>
@@ -2036,15 +2082,16 @@
       <c r="F35" s="22"/>
       <c r="G35" s="22"/>
       <c r="H35" s="15"/>
-      <c r="J35" s="13" t="s">
+      <c r="I35" s="32"/>
+      <c r="K35" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="K35" s="13"/>
-      <c r="L35" s="14" t="s">
+      <c r="L35" s="13"/>
+      <c r="M35" s="14" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
         <v>3</v>
       </c>
@@ -2056,16 +2103,17 @@
       <c r="E36" s="22"/>
       <c r="F36" s="22"/>
       <c r="G36" s="22"/>
-      <c r="H36" s="15"/>
-      <c r="J36" s="13" t="s">
+      <c r="H36" s="22"/>
+      <c r="I36" s="32"/>
+      <c r="K36" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="K36" s="13"/>
-      <c r="L36" s="14" t="s">
+      <c r="L36" s="13"/>
+      <c r="M36" s="14" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
         <v>4</v>
       </c>
@@ -2077,16 +2125,17 @@
       <c r="E37" s="22"/>
       <c r="F37" s="22"/>
       <c r="G37" s="22"/>
-      <c r="H37" s="15"/>
-      <c r="J37" s="13" t="s">
+      <c r="H37" s="22"/>
+      <c r="I37" s="32"/>
+      <c r="K37" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="K37" s="13"/>
-      <c r="L37" s="14" t="s">
+      <c r="L37" s="13"/>
+      <c r="M37" s="14" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
         <v>5</v>
       </c>
@@ -2099,15 +2148,16 @@
       <c r="F38" s="22"/>
       <c r="G38" s="22"/>
       <c r="H38" s="15"/>
-      <c r="J38" s="13" t="s">
+      <c r="I38" s="32"/>
+      <c r="K38" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="K38" s="13"/>
-      <c r="L38" s="14" t="s">
+      <c r="L38" s="13"/>
+      <c r="M38" s="14" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
         <v>6</v>
       </c>
@@ -2120,15 +2170,16 @@
       <c r="F39" s="22"/>
       <c r="G39" s="15"/>
       <c r="H39" s="15"/>
-      <c r="J39" s="13" t="s">
+      <c r="I39" s="32"/>
+      <c r="K39" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="K39" s="13"/>
-      <c r="L39" s="14" t="s">
+      <c r="L39" s="13"/>
+      <c r="M39" s="14" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
         <v>7</v>
       </c>
@@ -2141,17 +2192,18 @@
       <c r="F40" s="22"/>
       <c r="G40" s="15"/>
       <c r="H40" s="15"/>
-      <c r="J40" s="13" t="s">
+      <c r="I40" s="32"/>
+      <c r="K40" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="K40" s="13" t="s">
+      <c r="L40" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="L40" s="14" t="s">
+      <c r="M40" s="14" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="16">
         <v>8</v>
       </c>
@@ -2164,15 +2216,16 @@
       <c r="F41" s="22"/>
       <c r="G41" s="15"/>
       <c r="H41" s="15"/>
-      <c r="J41" s="13" t="s">
+      <c r="I41" s="32"/>
+      <c r="K41" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="K41" s="13"/>
-      <c r="L41" s="14" t="s">
+      <c r="L41" s="13"/>
+      <c r="M41" s="14" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="82.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" ht="99" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>122</v>
       </c>
@@ -2197,12 +2250,15 @@
       <c r="H44" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="I44" s="1"/>
+      <c r="I44" s="35" t="s">
+        <v>224</v>
+      </c>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
-    </row>
-    <row r="45" spans="1:13" ht="42" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M44" s="1"/>
+    </row>
+    <row r="45" spans="1:14" ht="42" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="10"/>
       <c r="B45" s="28">
         <v>2020</v>
@@ -2225,12 +2281,15 @@
       <c r="H45" s="7">
         <v>43951</v>
       </c>
-      <c r="I45" s="1"/>
+      <c r="I45" s="36">
+        <v>43928</v>
+      </c>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M45" s="1"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="11">
         <v>1</v>
       </c>
@@ -2243,15 +2302,16 @@
       <c r="F46" s="20"/>
       <c r="G46" s="20"/>
       <c r="H46" s="20"/>
-      <c r="J46" s="13" t="s">
+      <c r="I46" s="20"/>
+      <c r="K46" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="K46" s="13"/>
-      <c r="L46" s="14" t="s">
+      <c r="L46" s="13"/>
+      <c r="M46" s="14" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="12">
         <v>2</v>
       </c>
@@ -2264,15 +2324,16 @@
       <c r="F47" s="15"/>
       <c r="G47" s="15"/>
       <c r="H47" s="15"/>
-      <c r="J47" s="13" t="s">
+      <c r="I47" s="15"/>
+      <c r="K47" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="K47" s="13"/>
-      <c r="L47" s="14" t="s">
+      <c r="L47" s="13"/>
+      <c r="M47" s="14" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="12">
         <v>3</v>
       </c>
@@ -2285,17 +2346,18 @@
       <c r="F48" s="22"/>
       <c r="G48" s="15"/>
       <c r="H48" s="15"/>
-      <c r="J48" s="13" t="s">
+      <c r="I48" s="15"/>
+      <c r="K48" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="K48" s="13" t="s">
+      <c r="L48" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="L48" s="14" t="s">
+      <c r="M48" s="14" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="12">
         <v>4</v>
       </c>
@@ -2308,15 +2370,16 @@
       <c r="F49" s="22"/>
       <c r="G49" s="15"/>
       <c r="H49" s="15"/>
-      <c r="J49" s="13" t="s">
+      <c r="I49" s="15"/>
+      <c r="K49" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="K49" s="13"/>
-      <c r="L49" s="14" t="s">
+      <c r="L49" s="13"/>
+      <c r="M49" s="14" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="12">
         <v>5</v>
       </c>
@@ -2329,15 +2392,16 @@
       <c r="F50" s="22"/>
       <c r="G50" s="22"/>
       <c r="H50" s="15"/>
-      <c r="J50" s="13" t="s">
+      <c r="I50" s="15"/>
+      <c r="K50" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="K50" s="13"/>
-      <c r="L50" s="14" t="s">
+      <c r="L50" s="13"/>
+      <c r="M50" s="14" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="12">
         <v>6</v>
       </c>
@@ -2350,15 +2414,16 @@
       <c r="F51" s="22"/>
       <c r="G51" s="15"/>
       <c r="H51" s="15"/>
-      <c r="J51" s="13" t="s">
+      <c r="I51" s="15"/>
+      <c r="K51" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="K51" s="13"/>
-      <c r="L51" s="14" t="s">
+      <c r="L51" s="13"/>
+      <c r="M51" s="14" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="12">
         <v>7</v>
       </c>
@@ -2371,15 +2436,16 @@
       <c r="F52" s="22"/>
       <c r="G52" s="15"/>
       <c r="H52" s="15"/>
-      <c r="J52" s="13" t="s">
+      <c r="I52" s="15"/>
+      <c r="K52" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="K52" s="13"/>
-      <c r="L52" s="14" t="s">
+      <c r="L52" s="13"/>
+      <c r="M52" s="14" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="82.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" ht="99" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>122</v>
       </c>
@@ -2404,12 +2470,15 @@
       <c r="H55" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="I55" s="1"/>
+      <c r="I55" s="35" t="s">
+        <v>224</v>
+      </c>
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
       <c r="L55" s="1"/>
-    </row>
-    <row r="56" spans="1:12" ht="42" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M55" s="1"/>
+    </row>
+    <row r="56" spans="1:13" ht="42" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="10"/>
       <c r="B56" s="28">
         <v>2020</v>
@@ -2432,12 +2501,15 @@
       <c r="H56" s="7">
         <v>43951</v>
       </c>
-      <c r="I56" s="1"/>
+      <c r="I56" s="36">
+        <v>43928</v>
+      </c>
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M56" s="1"/>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
         <v>1</v>
       </c>
@@ -2450,15 +2522,16 @@
       <c r="F57" s="23"/>
       <c r="G57" s="20"/>
       <c r="H57" s="20"/>
-      <c r="J57" s="13" t="s">
+      <c r="I57" s="20"/>
+      <c r="K57" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="K57" s="13"/>
-      <c r="L57" s="14" t="s">
+      <c r="L57" s="13"/>
+      <c r="M57" s="14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="12">
         <v>2</v>
       </c>
@@ -2471,15 +2544,16 @@
       <c r="F58" s="22"/>
       <c r="G58" s="22"/>
       <c r="H58" s="22"/>
-      <c r="J58" s="13" t="s">
+      <c r="I58" s="22"/>
+      <c r="K58" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="K58" s="13"/>
-      <c r="L58" s="14" t="s">
+      <c r="L58" s="13"/>
+      <c r="M58" s="14" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="12">
         <v>3</v>
       </c>
@@ -2492,15 +2566,16 @@
       <c r="F59" s="22"/>
       <c r="G59" s="15"/>
       <c r="H59" s="15"/>
-      <c r="J59" s="13" t="s">
+      <c r="I59" s="22"/>
+      <c r="K59" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="K59" s="13"/>
-      <c r="L59" s="14" t="s">
+      <c r="L59" s="13"/>
+      <c r="M59" s="14" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="12">
         <v>4</v>
       </c>
@@ -2513,15 +2588,16 @@
       <c r="F60" s="15"/>
       <c r="G60" s="15"/>
       <c r="H60" s="15"/>
-      <c r="J60" s="13" t="s">
+      <c r="I60" s="15"/>
+      <c r="K60" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="K60" s="13"/>
-      <c r="L60" s="14" t="s">
+      <c r="L60" s="13"/>
+      <c r="M60" s="14" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="12">
         <v>5</v>
       </c>
@@ -2534,17 +2610,18 @@
       <c r="F61" s="22"/>
       <c r="G61" s="15"/>
       <c r="H61" s="15"/>
-      <c r="J61" s="13" t="s">
+      <c r="I61" s="15"/>
+      <c r="K61" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="K61" s="13" t="s">
+      <c r="L61" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="L61" s="14" t="s">
+      <c r="M61" s="14" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="12">
         <v>6</v>
       </c>
@@ -2556,16 +2633,17 @@
       <c r="E62" s="22"/>
       <c r="F62" s="22"/>
       <c r="G62" s="22"/>
-      <c r="H62" s="15"/>
-      <c r="J62" s="13" t="s">
+      <c r="H62" s="22"/>
+      <c r="I62" s="15"/>
+      <c r="K62" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="K62" s="13"/>
-      <c r="L62" s="14" t="s">
+      <c r="L62" s="13"/>
+      <c r="M62" s="14" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="12">
         <v>7</v>
       </c>
@@ -2578,15 +2656,16 @@
       <c r="F63" s="22"/>
       <c r="G63" s="22"/>
       <c r="H63" s="22"/>
-      <c r="J63" s="13" t="s">
+      <c r="I63" s="22"/>
+      <c r="K63" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="K63" s="13"/>
-      <c r="L63" s="14" t="s">
+      <c r="L63" s="13"/>
+      <c r="M63" s="14" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="16">
         <v>8</v>
       </c>
@@ -2599,15 +2678,16 @@
       <c r="F64" s="22"/>
       <c r="G64" s="22"/>
       <c r="H64" s="22"/>
-      <c r="J64" s="13" t="s">
+      <c r="I64" s="15"/>
+      <c r="K64" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="K64" s="13"/>
-      <c r="L64" s="14" t="s">
+      <c r="L64" s="13"/>
+      <c r="M64" s="14" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="16">
         <v>9</v>
       </c>
@@ -2620,15 +2700,16 @@
       <c r="F65" s="22"/>
       <c r="G65" s="22"/>
       <c r="H65" s="22"/>
-      <c r="J65" s="13" t="s">
+      <c r="I65" s="15"/>
+      <c r="K65" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="K65" s="13"/>
-      <c r="L65" s="14" t="s">
+      <c r="L65" s="13"/>
+      <c r="M65" s="14" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="17">
         <v>10</v>
       </c>
@@ -2640,14 +2721,15 @@
       <c r="E66" s="22"/>
       <c r="F66" s="15"/>
       <c r="G66" s="15"/>
-      <c r="H66" s="15"/>
-      <c r="J66" s="13" t="s">
+      <c r="H66" s="22"/>
+      <c r="I66" s="15"/>
+      <c r="K66" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="K66" s="13"/>
-      <c r="L66" s="14"/>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L66" s="13"/>
+      <c r="M66" s="14"/>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="17">
         <v>11</v>
       </c>
@@ -2658,17 +2740,18 @@
       <c r="D67" s="22"/>
       <c r="E67" s="22"/>
       <c r="F67" s="22"/>
-      <c r="G67" s="15"/>
-      <c r="H67" s="15"/>
-      <c r="J67" s="13" t="s">
+      <c r="G67" s="22"/>
+      <c r="H67" s="22"/>
+      <c r="I67" s="22"/>
+      <c r="K67" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="K67" s="13"/>
-      <c r="L67" s="14" t="s">
+      <c r="L67" s="13"/>
+      <c r="M67" s="14" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="82.5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" ht="99" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
         <v>122</v>
       </c>
@@ -2693,12 +2776,15 @@
       <c r="H70" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="I70" s="1"/>
+      <c r="I70" s="35" t="s">
+        <v>224</v>
+      </c>
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
       <c r="L70" s="1"/>
-    </row>
-    <row r="71" spans="1:12" ht="42" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M70" s="1"/>
+    </row>
+    <row r="71" spans="1:13" ht="42" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="10"/>
       <c r="B71" s="28">
         <v>2020</v>
@@ -2721,12 +2807,15 @@
       <c r="H71" s="7">
         <v>43951</v>
       </c>
-      <c r="I71" s="1"/>
+      <c r="I71" s="36">
+        <v>43928</v>
+      </c>
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
       <c r="L71" s="1"/>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M71" s="1"/>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="11">
         <v>1</v>
       </c>
@@ -2739,17 +2828,18 @@
       <c r="F72" s="23"/>
       <c r="G72" s="20"/>
       <c r="H72" s="4"/>
-      <c r="J72" s="13" t="s">
+      <c r="I72" s="20"/>
+      <c r="K72" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="K72" s="13" t="s">
+      <c r="L72" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="L72" s="14" t="s">
+      <c r="M72" s="14" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="17">
         <v>2</v>
       </c>
@@ -2762,14 +2852,15 @@
       <c r="F73" s="22"/>
       <c r="G73" s="22"/>
       <c r="H73" s="3"/>
-      <c r="J73" s="13" t="s">
+      <c r="I73" s="22"/>
+      <c r="K73" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="L73" s="14" t="s">
+      <c r="M73" s="14" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="12">
         <v>3</v>
       </c>
@@ -2782,15 +2873,16 @@
       <c r="F74" s="15"/>
       <c r="G74" s="15"/>
       <c r="H74" s="3"/>
-      <c r="J74" s="13" t="s">
+      <c r="I74" s="15"/>
+      <c r="K74" s="13" t="s">
         <v>171</v>
       </c>
-      <c r="K74" s="13"/>
-      <c r="L74" s="14" t="s">
+      <c r="L74" s="13"/>
+      <c r="M74" s="14" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="12">
         <v>4</v>
       </c>
@@ -2802,16 +2894,17 @@
       <c r="E75" s="15"/>
       <c r="F75" s="22"/>
       <c r="G75" s="22"/>
-      <c r="H75" s="3"/>
-      <c r="J75" s="13" t="s">
+      <c r="H75" s="22"/>
+      <c r="I75" s="15"/>
+      <c r="K75" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="K75" s="13"/>
-      <c r="L75" s="14" t="s">
+      <c r="L75" s="13"/>
+      <c r="M75" s="14" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="12">
         <v>5</v>
       </c>
@@ -2824,15 +2917,16 @@
       <c r="F76" s="22"/>
       <c r="G76" s="22"/>
       <c r="H76" s="3"/>
-      <c r="J76" s="13" t="s">
+      <c r="I76" s="15"/>
+      <c r="K76" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="K76" s="13"/>
-      <c r="L76" s="14" t="s">
+      <c r="L76" s="13"/>
+      <c r="M76" s="14" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="12">
         <v>6</v>
       </c>
@@ -2842,14 +2936,15 @@
       <c r="C77" s="25"/>
       <c r="D77" s="22"/>
       <c r="E77" s="15"/>
-      <c r="F77" s="15"/>
+      <c r="F77" s="22"/>
       <c r="G77" s="15"/>
       <c r="H77" s="3"/>
-      <c r="J77" s="13"/>
+      <c r="I77" s="15"/>
       <c r="K77" s="13"/>
-      <c r="L77" s="14"/>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L77" s="13"/>
+      <c r="M77" s="14"/>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="12">
         <v>7</v>
       </c>
@@ -2861,16 +2956,17 @@
       <c r="E78" s="22"/>
       <c r="F78" s="22"/>
       <c r="G78" s="22"/>
-      <c r="H78" s="3"/>
-      <c r="J78" s="13" t="s">
+      <c r="H78" s="22"/>
+      <c r="I78" s="15"/>
+      <c r="K78" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="K78" s="13"/>
-      <c r="L78" s="14" t="s">
+      <c r="L78" s="13"/>
+      <c r="M78" s="14" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="12">
         <v>8</v>
       </c>
@@ -2882,16 +2978,17 @@
       <c r="E79" s="3"/>
       <c r="F79" s="22"/>
       <c r="G79" s="22"/>
-      <c r="H79" s="3"/>
-      <c r="J79" s="13" t="s">
+      <c r="H79" s="22"/>
+      <c r="I79" s="15"/>
+      <c r="K79" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="K79" s="13"/>
-      <c r="L79" s="14" t="s">
+      <c r="L79" s="13"/>
+      <c r="M79" s="14" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="16">
         <v>9</v>
       </c>
@@ -2904,15 +3001,16 @@
       <c r="F80" s="22"/>
       <c r="G80" s="22"/>
       <c r="H80" s="3"/>
-      <c r="J80" s="13" t="s">
+      <c r="I80" s="15"/>
+      <c r="K80" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="K80" s="13"/>
-      <c r="L80" s="14" t="s">
+      <c r="L80" s="13"/>
+      <c r="M80" s="14" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="16">
         <v>10</v>
       </c>
@@ -2925,15 +3023,16 @@
       <c r="F81" s="22"/>
       <c r="G81" s="22"/>
       <c r="H81" s="3"/>
-      <c r="J81" s="13" t="s">
+      <c r="I81" s="15"/>
+      <c r="K81" s="13" t="s">
         <v>180</v>
       </c>
-      <c r="K81" s="13"/>
-      <c r="L81" s="14" t="s">
+      <c r="L81" s="13"/>
+      <c r="M81" s="14" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="17">
         <v>11</v>
       </c>
@@ -2946,15 +3045,16 @@
       <c r="F82" s="22"/>
       <c r="G82" s="22"/>
       <c r="H82" s="3"/>
-      <c r="J82" s="13" t="s">
+      <c r="I82" s="15"/>
+      <c r="K82" s="13" t="s">
         <v>182</v>
       </c>
-      <c r="K82" s="13"/>
-      <c r="L82" s="14" t="s">
+      <c r="L82" s="13"/>
+      <c r="M82" s="14" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="17">
         <v>12</v>
       </c>
@@ -2967,15 +3067,16 @@
       <c r="F83" s="22"/>
       <c r="G83" s="22"/>
       <c r="H83" s="3"/>
-      <c r="J83" s="13" t="s">
+      <c r="I83" s="15"/>
+      <c r="K83" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="K83" s="13"/>
-      <c r="L83" s="14" t="s">
+      <c r="L83" s="13"/>
+      <c r="M83" s="14" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" s="17">
         <v>13</v>
       </c>
@@ -2988,17 +3089,18 @@
       <c r="F84" s="22"/>
       <c r="G84" s="22"/>
       <c r="H84" s="3"/>
-      <c r="J84" s="13" t="s">
+      <c r="I84" s="15"/>
+      <c r="K84" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="K84" s="13" t="s">
+      <c r="L84" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="L84" s="14" t="s">
+      <c r="M84" s="14" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" s="17">
         <v>14</v>
       </c>
@@ -3011,14 +3113,15 @@
       <c r="F85" s="22"/>
       <c r="G85" s="22"/>
       <c r="H85" s="3"/>
-      <c r="J85" s="13" t="s">
+      <c r="I85" s="15"/>
+      <c r="K85" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="L85" s="14" t="s">
+      <c r="M85" s="14" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="88" spans="1:12" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
         <v>122</v>
       </c>
@@ -3037,12 +3140,13 @@
       <c r="F88" s="2"/>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
-      <c r="I88" s="1"/>
+      <c r="I88" s="33"/>
       <c r="J88" s="1"/>
       <c r="K88" s="1"/>
       <c r="L88" s="1"/>
-    </row>
-    <row r="89" spans="1:12" ht="42" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M88" s="1"/>
+    </row>
+    <row r="89" spans="1:13" ht="42" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="10"/>
       <c r="B89" s="28">
         <v>2020</v>
@@ -3059,12 +3163,13 @@
       <c r="F89" s="8"/>
       <c r="G89" s="8"/>
       <c r="H89" s="8"/>
-      <c r="I89" s="1"/>
+      <c r="I89" s="34"/>
       <c r="J89" s="1"/>
       <c r="K89" s="1"/>
       <c r="L89" s="1"/>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M89" s="1"/>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" s="11">
         <v>1</v>
       </c>
@@ -3077,15 +3182,16 @@
       <c r="F90" s="20"/>
       <c r="G90" s="20"/>
       <c r="H90" s="20"/>
-      <c r="J90" s="13" t="s">
+      <c r="I90" s="32"/>
+      <c r="K90" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="K90" s="13"/>
-      <c r="L90" s="14" t="s">
+      <c r="L90" s="13"/>
+      <c r="M90" s="14" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" s="12">
         <v>2</v>
       </c>
@@ -3098,15 +3204,16 @@
       <c r="F91" s="15"/>
       <c r="G91" s="15"/>
       <c r="H91" s="15"/>
-      <c r="J91" s="13" t="s">
+      <c r="I91" s="32"/>
+      <c r="K91" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="K91" s="13"/>
-      <c r="L91" s="14" t="s">
+      <c r="L91" s="13"/>
+      <c r="M91" s="14" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" s="12">
         <v>3</v>
       </c>
@@ -3119,15 +3226,16 @@
       <c r="F92" s="15"/>
       <c r="G92" s="15"/>
       <c r="H92" s="15"/>
-      <c r="J92" s="13" t="s">
+      <c r="I92" s="32"/>
+      <c r="K92" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="K92" s="13"/>
-      <c r="L92" s="14" t="s">
+      <c r="L92" s="13"/>
+      <c r="M92" s="14" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" s="12">
         <v>4</v>
       </c>
@@ -3140,17 +3248,18 @@
       <c r="F93" s="15"/>
       <c r="G93" s="15"/>
       <c r="H93" s="15"/>
-      <c r="J93" s="13" t="s">
+      <c r="I93" s="32"/>
+      <c r="K93" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="K93" s="13" t="s">
+      <c r="L93" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="L93" s="14" t="s">
+      <c r="M93" s="14" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" s="12">
         <v>5</v>
       </c>
@@ -3163,14 +3272,15 @@
       <c r="F94" s="15"/>
       <c r="G94" s="15"/>
       <c r="H94" s="15"/>
-      <c r="J94" s="13" t="s">
+      <c r="I94" s="32"/>
+      <c r="K94" s="13" t="s">
         <v>205</v>
       </c>
-      <c r="L94" s="14" t="s">
+      <c r="M94" s="14" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" s="12">
         <v>6</v>
       </c>
@@ -3183,81 +3293,82 @@
       <c r="F95" s="15"/>
       <c r="G95" s="15"/>
       <c r="H95" s="15"/>
-      <c r="J95" s="13" t="s">
+      <c r="I95" s="32"/>
+      <c r="K95" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="K95" s="13"/>
-      <c r="L95" s="14" t="s">
+      <c r="L95" s="13"/>
+      <c r="M95" s="14" t="s">
         <v>208</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L4" r:id="rId1" xr:uid="{AE0A5EED-E877-47F1-95C6-BFD4B992DCBE}"/>
-    <hyperlink ref="L5" r:id="rId2" xr:uid="{5AF98C2D-54A1-4433-A225-8EDA251E9782}"/>
-    <hyperlink ref="L6" r:id="rId3" xr:uid="{3BC9A1BA-B262-4227-8230-EFAFD41E9AE5}"/>
-    <hyperlink ref="L8" r:id="rId4" xr:uid="{1B3ECF74-0B44-4145-8ACA-5045787D820A}"/>
-    <hyperlink ref="L9" r:id="rId5" xr:uid="{38D8D2C0-99A0-43BE-B10C-8466CD0AEC0B}"/>
-    <hyperlink ref="L10" r:id="rId6" xr:uid="{24A4A094-2EC6-4AD2-9AC2-914048976E4A}"/>
-    <hyperlink ref="L11" r:id="rId7" xr:uid="{FAFECAD6-1904-44BB-BFE4-85ACEE9BFDE9}"/>
-    <hyperlink ref="L12" r:id="rId8" xr:uid="{C8852359-C5FE-4964-8FCE-9A90470981AA}"/>
-    <hyperlink ref="L7" r:id="rId9" xr:uid="{42CCD745-D6E9-4CB3-98ED-698D7775388D}"/>
-    <hyperlink ref="L17" r:id="rId10" xr:uid="{296994C2-7C61-4A7D-9F6F-3F68BD3D88C8}"/>
-    <hyperlink ref="L18" r:id="rId11" xr:uid="{366FBF39-E99D-4BD8-A888-68090C5AAB58}"/>
-    <hyperlink ref="L19" r:id="rId12" xr:uid="{C4D3AC60-B676-405A-999C-6D0BF36ADED4}"/>
-    <hyperlink ref="L21" r:id="rId13" xr:uid="{D056DB16-14E8-4139-BFBC-E689F4833646}"/>
-    <hyperlink ref="L22" r:id="rId14" xr:uid="{E9757565-0EC0-4CCA-8717-DD82F92D5BE5}"/>
-    <hyperlink ref="L23" r:id="rId15" xr:uid="{ECD78E6D-1DE0-4330-B8D5-B9C13121A6AB}"/>
-    <hyperlink ref="L24" r:id="rId16" xr:uid="{0E1136CC-BA1C-42C8-A639-D9B32A05E06C}"/>
-    <hyperlink ref="L25" r:id="rId17" xr:uid="{5CD4DE1A-1AEF-4258-B1CC-D4F89EBB2C6B}"/>
-    <hyperlink ref="L20" r:id="rId18" xr:uid="{85BD47E5-3027-424E-8EA5-63AFFCC79798}"/>
-    <hyperlink ref="L27" r:id="rId19" xr:uid="{429ECF84-3F17-453F-A8CD-FF5BB02F2C6E}"/>
-    <hyperlink ref="L29" r:id="rId20" xr:uid="{0FE4A098-5FFB-469E-B3D1-D7935DBDA769}"/>
-    <hyperlink ref="L34" r:id="rId21" xr:uid="{7666C554-894B-4540-90BF-A722F3355CC4}"/>
-    <hyperlink ref="L35" r:id="rId22" xr:uid="{69538AF5-D004-4BEB-97EC-EB9C44374090}"/>
-    <hyperlink ref="L36" r:id="rId23" xr:uid="{420F4813-1972-4E64-A982-ADA5E552B377}"/>
-    <hyperlink ref="L38" r:id="rId24" xr:uid="{EC86E1E1-6571-4A83-8A1D-A983BB036B1E}"/>
-    <hyperlink ref="L39" r:id="rId25" xr:uid="{16EBDAED-8A87-4584-B7D7-2887F94F81B1}"/>
-    <hyperlink ref="L40" r:id="rId26" xr:uid="{DD5A28AB-4507-4879-A577-695129FACBE0}"/>
-    <hyperlink ref="L41" r:id="rId27" xr:uid="{25CBFEB8-5CD6-4191-B7DF-DB3EF95DF242}"/>
-    <hyperlink ref="L37" r:id="rId28" xr:uid="{7C409F90-A335-4A77-9A97-A3BB765CE416}"/>
-    <hyperlink ref="M34" r:id="rId29" xr:uid="{F913FCC3-8AA8-4712-9550-63A79A632B66}"/>
-    <hyperlink ref="L46" r:id="rId30" xr:uid="{12401ABD-5BA9-40B9-8A98-F6E39B148C3B}"/>
-    <hyperlink ref="L47" r:id="rId31" xr:uid="{AF3A57FD-40EF-46EC-B641-DAEF2A50072A}"/>
-    <hyperlink ref="L48" r:id="rId32" xr:uid="{24792718-4D53-4BE7-ABC5-5E465087308B}"/>
-    <hyperlink ref="L50" r:id="rId33" xr:uid="{4D9FB32D-95E6-40B7-876E-CFA736652C2C}"/>
-    <hyperlink ref="L51" r:id="rId34" xr:uid="{6996CF09-5936-4A11-BCE6-4E07E56E161F}"/>
-    <hyperlink ref="L52" r:id="rId35" xr:uid="{2789BF76-D066-47BA-915F-41451578DF98}"/>
-    <hyperlink ref="L49" r:id="rId36" xr:uid="{568AD010-D627-4475-89F9-8F227E649F87}"/>
-    <hyperlink ref="L57" r:id="rId37" xr:uid="{0B7B1FE0-457A-4D24-8FFE-247BAADDEF1D}"/>
-    <hyperlink ref="L58" r:id="rId38" xr:uid="{47C5B8F0-CA12-4371-B567-F6CFFC886BB1}"/>
-    <hyperlink ref="L59" r:id="rId39" xr:uid="{153797E4-E21F-4DF1-A95A-1C1390B81B93}"/>
-    <hyperlink ref="L61" r:id="rId40" xr:uid="{53E48E75-7DF9-4FA3-8E37-AAC0E9E51728}"/>
-    <hyperlink ref="L62" r:id="rId41" xr:uid="{771E4588-E60D-41E5-9EB1-AB6780B56CB3}"/>
-    <hyperlink ref="L63" r:id="rId42" xr:uid="{313D817E-2E75-47AA-8E2B-EE178E69E72B}"/>
-    <hyperlink ref="L64" r:id="rId43" xr:uid="{9FCF0F96-85B5-4DB8-B3E8-6E5AAF72575B}"/>
-    <hyperlink ref="L65" r:id="rId44" xr:uid="{14274367-6B0C-4F46-8AF7-BE44A88610DA}"/>
-    <hyperlink ref="L60" r:id="rId45" xr:uid="{B060C748-0A75-43B2-8148-EA9539BEDA6C}"/>
-    <hyperlink ref="L67" r:id="rId46" xr:uid="{9337F166-DBED-4D36-BEFF-5F314FBC92C4}"/>
-    <hyperlink ref="L72" r:id="rId47" xr:uid="{D6A35461-8F4E-48A3-BCC2-8452A007F42F}"/>
-    <hyperlink ref="L74" r:id="rId48" xr:uid="{A1E15E18-865A-428D-BD73-4D7854A3F882}"/>
-    <hyperlink ref="L75" r:id="rId49" xr:uid="{FC4A0CF8-E5E5-4A69-A79A-BE581DE1B753}"/>
-    <hyperlink ref="L78" r:id="rId50" xr:uid="{FA1EEF9B-8870-4C99-ABA1-FFCDFC67258F}"/>
-    <hyperlink ref="L79" r:id="rId51" xr:uid="{6DF3237B-F457-48C8-9ACA-51051688FE23}"/>
-    <hyperlink ref="L80" r:id="rId52" xr:uid="{62C9B97A-2788-4F90-AA2A-579EC1BD7CEF}"/>
-    <hyperlink ref="L81" r:id="rId53" xr:uid="{B63B3740-BF73-4EB4-8635-B589531BBB36}"/>
-    <hyperlink ref="L76" r:id="rId54" xr:uid="{59C18176-78F0-4E26-8E5F-69C860CABC51}"/>
-    <hyperlink ref="L83" r:id="rId55" xr:uid="{7A459DA2-0FC2-4564-9A81-8B699BFD551F}"/>
-    <hyperlink ref="L82" r:id="rId56" xr:uid="{7B6C5D0A-9805-4C5D-8CCC-4049D2B4396F}"/>
-    <hyperlink ref="L84" r:id="rId57" xr:uid="{22AE91FC-178D-43F2-9391-FD91305E2C3A}"/>
-    <hyperlink ref="L85" r:id="rId58" xr:uid="{8AF0D46F-6402-495B-9DB4-95C4115C5BF3}"/>
-    <hyperlink ref="L73" r:id="rId59" xr:uid="{0589E4C5-E0F8-4D62-810B-5A2493891FA7}"/>
-    <hyperlink ref="L90" r:id="rId60" xr:uid="{D88FBCC2-E2E1-46EA-A873-4913F32E563D}"/>
-    <hyperlink ref="L91" r:id="rId61" xr:uid="{A877EDB9-FFDB-4C1E-9598-EE8A41A1DDE5}"/>
-    <hyperlink ref="L92" r:id="rId62" xr:uid="{97B73E21-A956-4577-85E7-3BFE1A5499DA}"/>
-    <hyperlink ref="L94" r:id="rId63" xr:uid="{21CD9E27-A5CE-4C8A-9537-B717BD2CACCC}"/>
-    <hyperlink ref="L95" r:id="rId64" xr:uid="{823665A7-821A-4643-AEDC-8AE4D6B1F8B7}"/>
-    <hyperlink ref="L93" r:id="rId65" xr:uid="{197354A2-B6D6-47E9-B520-B865F7918954}"/>
+    <hyperlink ref="M4" r:id="rId1" xr:uid="{AE0A5EED-E877-47F1-95C6-BFD4B992DCBE}"/>
+    <hyperlink ref="M5" r:id="rId2" xr:uid="{5AF98C2D-54A1-4433-A225-8EDA251E9782}"/>
+    <hyperlink ref="M6" r:id="rId3" xr:uid="{3BC9A1BA-B262-4227-8230-EFAFD41E9AE5}"/>
+    <hyperlink ref="M8" r:id="rId4" xr:uid="{1B3ECF74-0B44-4145-8ACA-5045787D820A}"/>
+    <hyperlink ref="M9" r:id="rId5" xr:uid="{38D8D2C0-99A0-43BE-B10C-8466CD0AEC0B}"/>
+    <hyperlink ref="M10" r:id="rId6" xr:uid="{24A4A094-2EC6-4AD2-9AC2-914048976E4A}"/>
+    <hyperlink ref="M11" r:id="rId7" xr:uid="{FAFECAD6-1904-44BB-BFE4-85ACEE9BFDE9}"/>
+    <hyperlink ref="M12" r:id="rId8" xr:uid="{C8852359-C5FE-4964-8FCE-9A90470981AA}"/>
+    <hyperlink ref="M7" r:id="rId9" xr:uid="{42CCD745-D6E9-4CB3-98ED-698D7775388D}"/>
+    <hyperlink ref="M17" r:id="rId10" xr:uid="{296994C2-7C61-4A7D-9F6F-3F68BD3D88C8}"/>
+    <hyperlink ref="M18" r:id="rId11" xr:uid="{366FBF39-E99D-4BD8-A888-68090C5AAB58}"/>
+    <hyperlink ref="M19" r:id="rId12" xr:uid="{C4D3AC60-B676-405A-999C-6D0BF36ADED4}"/>
+    <hyperlink ref="M21" r:id="rId13" xr:uid="{D056DB16-14E8-4139-BFBC-E689F4833646}"/>
+    <hyperlink ref="M22" r:id="rId14" xr:uid="{E9757565-0EC0-4CCA-8717-DD82F92D5BE5}"/>
+    <hyperlink ref="M23" r:id="rId15" xr:uid="{ECD78E6D-1DE0-4330-B8D5-B9C13121A6AB}"/>
+    <hyperlink ref="M24" r:id="rId16" xr:uid="{0E1136CC-BA1C-42C8-A639-D9B32A05E06C}"/>
+    <hyperlink ref="M25" r:id="rId17" xr:uid="{5CD4DE1A-1AEF-4258-B1CC-D4F89EBB2C6B}"/>
+    <hyperlink ref="M20" r:id="rId18" xr:uid="{85BD47E5-3027-424E-8EA5-63AFFCC79798}"/>
+    <hyperlink ref="M27" r:id="rId19" xr:uid="{429ECF84-3F17-453F-A8CD-FF5BB02F2C6E}"/>
+    <hyperlink ref="M29" r:id="rId20" xr:uid="{0FE4A098-5FFB-469E-B3D1-D7935DBDA769}"/>
+    <hyperlink ref="M34" r:id="rId21" xr:uid="{7666C554-894B-4540-90BF-A722F3355CC4}"/>
+    <hyperlink ref="M35" r:id="rId22" xr:uid="{69538AF5-D004-4BEB-97EC-EB9C44374090}"/>
+    <hyperlink ref="M36" r:id="rId23" xr:uid="{420F4813-1972-4E64-A982-ADA5E552B377}"/>
+    <hyperlink ref="M38" r:id="rId24" xr:uid="{EC86E1E1-6571-4A83-8A1D-A983BB036B1E}"/>
+    <hyperlink ref="M39" r:id="rId25" xr:uid="{16EBDAED-8A87-4584-B7D7-2887F94F81B1}"/>
+    <hyperlink ref="M40" r:id="rId26" xr:uid="{DD5A28AB-4507-4879-A577-695129FACBE0}"/>
+    <hyperlink ref="M41" r:id="rId27" xr:uid="{25CBFEB8-5CD6-4191-B7DF-DB3EF95DF242}"/>
+    <hyperlink ref="M37" r:id="rId28" xr:uid="{7C409F90-A335-4A77-9A97-A3BB765CE416}"/>
+    <hyperlink ref="N34" r:id="rId29" xr:uid="{F913FCC3-8AA8-4712-9550-63A79A632B66}"/>
+    <hyperlink ref="M46" r:id="rId30" xr:uid="{12401ABD-5BA9-40B9-8A98-F6E39B148C3B}"/>
+    <hyperlink ref="M47" r:id="rId31" xr:uid="{AF3A57FD-40EF-46EC-B641-DAEF2A50072A}"/>
+    <hyperlink ref="M48" r:id="rId32" xr:uid="{24792718-4D53-4BE7-ABC5-5E465087308B}"/>
+    <hyperlink ref="M50" r:id="rId33" xr:uid="{4D9FB32D-95E6-40B7-876E-CFA736652C2C}"/>
+    <hyperlink ref="M51" r:id="rId34" xr:uid="{6996CF09-5936-4A11-BCE6-4E07E56E161F}"/>
+    <hyperlink ref="M52" r:id="rId35" xr:uid="{2789BF76-D066-47BA-915F-41451578DF98}"/>
+    <hyperlink ref="M49" r:id="rId36" xr:uid="{568AD010-D627-4475-89F9-8F227E649F87}"/>
+    <hyperlink ref="M57" r:id="rId37" xr:uid="{0B7B1FE0-457A-4D24-8FFE-247BAADDEF1D}"/>
+    <hyperlink ref="M58" r:id="rId38" xr:uid="{47C5B8F0-CA12-4371-B567-F6CFFC886BB1}"/>
+    <hyperlink ref="M59" r:id="rId39" xr:uid="{153797E4-E21F-4DF1-A95A-1C1390B81B93}"/>
+    <hyperlink ref="M61" r:id="rId40" xr:uid="{53E48E75-7DF9-4FA3-8E37-AAC0E9E51728}"/>
+    <hyperlink ref="M62" r:id="rId41" xr:uid="{771E4588-E60D-41E5-9EB1-AB6780B56CB3}"/>
+    <hyperlink ref="M63" r:id="rId42" xr:uid="{313D817E-2E75-47AA-8E2B-EE178E69E72B}"/>
+    <hyperlink ref="M64" r:id="rId43" xr:uid="{9FCF0F96-85B5-4DB8-B3E8-6E5AAF72575B}"/>
+    <hyperlink ref="M65" r:id="rId44" xr:uid="{14274367-6B0C-4F46-8AF7-BE44A88610DA}"/>
+    <hyperlink ref="M60" r:id="rId45" xr:uid="{B060C748-0A75-43B2-8148-EA9539BEDA6C}"/>
+    <hyperlink ref="M67" r:id="rId46" xr:uid="{9337F166-DBED-4D36-BEFF-5F314FBC92C4}"/>
+    <hyperlink ref="M72" r:id="rId47" xr:uid="{D6A35461-8F4E-48A3-BCC2-8452A007F42F}"/>
+    <hyperlink ref="M74" r:id="rId48" xr:uid="{A1E15E18-865A-428D-BD73-4D7854A3F882}"/>
+    <hyperlink ref="M75" r:id="rId49" xr:uid="{FC4A0CF8-E5E5-4A69-A79A-BE581DE1B753}"/>
+    <hyperlink ref="M78" r:id="rId50" xr:uid="{FA1EEF9B-8870-4C99-ABA1-FFCDFC67258F}"/>
+    <hyperlink ref="M79" r:id="rId51" xr:uid="{6DF3237B-F457-48C8-9ACA-51051688FE23}"/>
+    <hyperlink ref="M80" r:id="rId52" xr:uid="{62C9B97A-2788-4F90-AA2A-579EC1BD7CEF}"/>
+    <hyperlink ref="M81" r:id="rId53" xr:uid="{B63B3740-BF73-4EB4-8635-B589531BBB36}"/>
+    <hyperlink ref="M76" r:id="rId54" xr:uid="{59C18176-78F0-4E26-8E5F-69C860CABC51}"/>
+    <hyperlink ref="M83" r:id="rId55" xr:uid="{7A459DA2-0FC2-4564-9A81-8B699BFD551F}"/>
+    <hyperlink ref="M82" r:id="rId56" xr:uid="{7B6C5D0A-9805-4C5D-8CCC-4049D2B4396F}"/>
+    <hyperlink ref="M84" r:id="rId57" xr:uid="{22AE91FC-178D-43F2-9391-FD91305E2C3A}"/>
+    <hyperlink ref="M85" r:id="rId58" xr:uid="{8AF0D46F-6402-495B-9DB4-95C4115C5BF3}"/>
+    <hyperlink ref="M73" r:id="rId59" xr:uid="{0589E4C5-E0F8-4D62-810B-5A2493891FA7}"/>
+    <hyperlink ref="M90" r:id="rId60" xr:uid="{D88FBCC2-E2E1-46EA-A873-4913F32E563D}"/>
+    <hyperlink ref="M91" r:id="rId61" xr:uid="{A877EDB9-FFDB-4C1E-9598-EE8A41A1DDE5}"/>
+    <hyperlink ref="M92" r:id="rId62" xr:uid="{97B73E21-A956-4577-85E7-3BFE1A5499DA}"/>
+    <hyperlink ref="M94" r:id="rId63" xr:uid="{21CD9E27-A5CE-4C8A-9537-B717BD2CACCC}"/>
+    <hyperlink ref="M95" r:id="rId64" xr:uid="{823665A7-821A-4643-AEDC-8AE4D6B1F8B7}"/>
+    <hyperlink ref="M93" r:id="rId65" xr:uid="{197354A2-B6D6-47E9-B520-B865F7918954}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId66"/>

</xml_diff>

<commit_message>
05.12 new files added
</commit_message>
<xml_diff>
--- a/Gyerekek.xlsx
+++ b/Gyerekek.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Privat\Informatika\Github\ZitaTuroczi1.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC273282-A490-43F5-BE10-EB29EFBF8488}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53298A03-D273-4323-A073-64A1B5EDB037}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12735" yWindow="330" windowWidth="13455" windowHeight="14865" xr2:uid="{D8DA68CD-37D4-4C3C-BD5C-8E37EBBBD311}"/>
+    <workbookView xWindow="13080" yWindow="675" windowWidth="13455" windowHeight="14865" xr2:uid="{D8DA68CD-37D4-4C3C-BD5C-8E37EBBBD311}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="226">
   <si>
     <t xml:space="preserve">Előképző 
 </t>
@@ -707,6 +707,9 @@
   </si>
   <si>
     <t>Pillangó hajtogatása</t>
+  </si>
+  <si>
+    <t>Ceruzatartó készítése</t>
   </si>
 </sst>
 </file>
@@ -1360,8 +1363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9286C3FF-60BE-42C4-89D5-9ACF7C2ACF54}">
   <dimension ref="A2:N95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L63" sqref="L63"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K98" sqref="K98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1888,7 +1891,7 @@
       <c r="E25" s="22"/>
       <c r="F25" s="22"/>
       <c r="G25" s="22"/>
-      <c r="H25" s="3"/>
+      <c r="H25" s="22"/>
       <c r="I25" s="32"/>
       <c r="K25" s="13" t="s">
         <v>66</v>
@@ -1930,7 +1933,7 @@
       <c r="E27" s="22"/>
       <c r="F27" s="22"/>
       <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
+      <c r="H27" s="22"/>
       <c r="I27" s="32"/>
       <c r="K27" s="13" t="s">
         <v>69</v>
@@ -1954,7 +1957,7 @@
       <c r="E28" s="22"/>
       <c r="F28" s="22"/>
       <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
+      <c r="H28" s="22"/>
       <c r="I28" s="32"/>
       <c r="K28" s="13"/>
       <c r="L28" s="13"/>
@@ -2168,7 +2171,7 @@
       <c r="D39" s="22"/>
       <c r="E39" s="22"/>
       <c r="F39" s="22"/>
-      <c r="G39" s="15"/>
+      <c r="G39" s="22"/>
       <c r="H39" s="15"/>
       <c r="I39" s="32"/>
       <c r="K39" s="13" t="s">
@@ -3121,7 +3124,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="88" spans="1:13" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
         <v>122</v>
       </c>
@@ -3137,7 +3140,9 @@
       <c r="E88" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="F88" s="2"/>
+      <c r="F88" s="2" t="s">
+        <v>225</v>
+      </c>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
       <c r="I88" s="33"/>
@@ -3160,7 +3165,9 @@
       <c r="E89" s="8">
         <v>43949</v>
       </c>
-      <c r="F89" s="8"/>
+      <c r="F89" s="8">
+        <v>43963</v>
+      </c>
       <c r="G89" s="8"/>
       <c r="H89" s="8"/>
       <c r="I89" s="34"/>

</xml_diff>

<commit_message>
A5-E2 feladatokhoz rajzok added
</commit_message>
<xml_diff>
--- a/Gyerekek.xlsx
+++ b/Gyerekek.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Privat\Informatika\Github\ZitaTuroczi1.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE049D1-303B-4EED-B0D5-FD621E4F1968}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1AF33D0-CEDD-4906-9B04-AACDA9401DC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14955" yWindow="75" windowWidth="13260" windowHeight="14865" xr2:uid="{D8DA68CD-37D4-4C3C-BD5C-8E37EBBBD311}"/>
+    <workbookView xWindow="19170" yWindow="60" windowWidth="9045" windowHeight="14880" xr2:uid="{D8DA68CD-37D4-4C3C-BD5C-8E37EBBBD311}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -761,7 +761,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -972,12 +972,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
@@ -1049,6 +1058,20 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hivatkozás" xfId="1" builtinId="8"/>
@@ -1364,10 +1387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9286C3FF-60BE-42C4-89D5-9ACF7C2ACF54}">
-  <dimension ref="A2:O95"/>
+  <dimension ref="A2:O96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J88" sqref="J88"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3232,8 +3255,8 @@
       <c r="F88" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="G88" s="2"/>
-      <c r="H88" s="2"/>
+      <c r="G88" s="40"/>
+      <c r="H88" s="37"/>
       <c r="I88" s="33"/>
       <c r="J88" s="33"/>
       <c r="K88" s="1"/>
@@ -3258,8 +3281,8 @@
       <c r="F89" s="8">
         <v>43963</v>
       </c>
-      <c r="G89" s="8"/>
-      <c r="H89" s="8"/>
+      <c r="G89" s="41"/>
+      <c r="H89" s="38"/>
       <c r="I89" s="34"/>
       <c r="J89" s="34"/>
       <c r="K89" s="1"/>
@@ -3278,8 +3301,8 @@
       <c r="D90" s="20"/>
       <c r="E90" s="20"/>
       <c r="F90" s="20"/>
-      <c r="G90" s="20"/>
-      <c r="H90" s="20"/>
+      <c r="G90" s="42"/>
+      <c r="H90" s="32"/>
       <c r="I90" s="32"/>
       <c r="J90" s="32"/>
       <c r="L90" s="13" t="s">
@@ -3301,8 +3324,8 @@
       <c r="D91" s="22"/>
       <c r="E91" s="22"/>
       <c r="F91" s="15"/>
-      <c r="G91" s="15"/>
-      <c r="H91" s="15"/>
+      <c r="G91" s="42"/>
+      <c r="H91" s="32"/>
       <c r="I91" s="32"/>
       <c r="J91" s="32"/>
       <c r="L91" s="13" t="s">
@@ -3324,8 +3347,8 @@
       <c r="D92" s="15"/>
       <c r="E92" s="15"/>
       <c r="F92" s="15"/>
-      <c r="G92" s="15"/>
-      <c r="H92" s="15"/>
+      <c r="G92" s="42"/>
+      <c r="H92" s="32"/>
       <c r="I92" s="32"/>
       <c r="J92" s="32"/>
       <c r="L92" s="13" t="s">
@@ -3347,8 +3370,8 @@
       <c r="D93" s="22"/>
       <c r="E93" s="22"/>
       <c r="F93" s="15"/>
-      <c r="G93" s="15"/>
-      <c r="H93" s="15"/>
+      <c r="G93" s="42"/>
+      <c r="H93" s="32"/>
       <c r="I93" s="32"/>
       <c r="J93" s="32"/>
       <c r="L93" s="13" t="s">
@@ -3372,8 +3395,8 @@
       <c r="D94" s="22"/>
       <c r="E94" s="22"/>
       <c r="F94" s="15"/>
-      <c r="G94" s="15"/>
-      <c r="H94" s="15"/>
+      <c r="G94" s="42"/>
+      <c r="H94" s="32"/>
       <c r="I94" s="32"/>
       <c r="J94" s="32"/>
       <c r="L94" s="13" t="s">
@@ -3394,8 +3417,8 @@
       <c r="D95" s="22"/>
       <c r="E95" s="22"/>
       <c r="F95" s="15"/>
-      <c r="G95" s="15"/>
-      <c r="H95" s="15"/>
+      <c r="G95" s="42"/>
+      <c r="H95" s="32"/>
       <c r="I95" s="32"/>
       <c r="J95" s="32"/>
       <c r="L95" s="13" t="s">
@@ -3405,6 +3428,11 @@
       <c r="N95" s="14" t="s">
         <v>208</v>
       </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H96" s="39"/>
+      <c r="I96" s="32"/>
+      <c r="J96" s="32"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
05.17 new pictures added + HermanNora corrected
</commit_message>
<xml_diff>
--- a/Gyerekek.xlsx
+++ b/Gyerekek.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Privat\Informatika\Github\ZitaTuroczi1.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{929E1F5F-7392-4345-98A7-D130F296E9E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F5A7D2-1870-4F33-9CCE-872B4E9BB744}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="15" windowWidth="9045" windowHeight="14880" xr2:uid="{D8DA68CD-37D4-4C3C-BD5C-8E37EBBBD311}"/>
+    <workbookView xWindow="18810" yWindow="555" windowWidth="9045" windowHeight="14880" xr2:uid="{D8DA68CD-37D4-4C3C-BD5C-8E37EBBBD311}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -1389,8 +1389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9286C3FF-60BE-42C4-89D5-9ACF7C2ACF54}">
   <dimension ref="A2:O96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1489,12 +1489,12 @@
       <c r="B5" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="21"/>
+      <c r="C5" s="25"/>
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
       <c r="F5" s="22"/>
       <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
+      <c r="H5" s="22"/>
       <c r="I5" s="32"/>
       <c r="J5" s="32"/>
       <c r="L5" s="13" t="s">
@@ -1961,7 +1961,7 @@
       <c r="E26" s="22"/>
       <c r="F26" s="22"/>
       <c r="G26" s="22"/>
-      <c r="H26" s="3"/>
+      <c r="H26" s="22"/>
       <c r="I26" s="32"/>
       <c r="J26" s="32"/>
       <c r="L26" s="13" t="s">
@@ -2111,7 +2111,7 @@
       <c r="E34" s="23"/>
       <c r="F34" s="23"/>
       <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
+      <c r="H34" s="23"/>
       <c r="I34" s="32"/>
       <c r="J34" s="32"/>
       <c r="L34" s="13" t="s">
@@ -2231,7 +2231,7 @@
       <c r="E39" s="22"/>
       <c r="F39" s="22"/>
       <c r="G39" s="22"/>
-      <c r="H39" s="15"/>
+      <c r="H39" s="22"/>
       <c r="I39" s="32"/>
       <c r="J39" s="32"/>
       <c r="L39" s="13" t="s">
@@ -2630,7 +2630,7 @@
       <c r="G58" s="22"/>
       <c r="H58" s="22"/>
       <c r="I58" s="22"/>
-      <c r="J58" s="15"/>
+      <c r="J58" s="22"/>
       <c r="L58" s="13" t="s">
         <v>135</v>
       </c>
@@ -2747,7 +2747,7 @@
       <c r="G63" s="22"/>
       <c r="H63" s="22"/>
       <c r="I63" s="22"/>
-      <c r="J63" s="15"/>
+      <c r="J63" s="22"/>
       <c r="L63" s="13" t="s">
         <v>66</v>
       </c>
@@ -2953,7 +2953,7 @@
       <c r="E73" s="3"/>
       <c r="F73" s="22"/>
       <c r="G73" s="22"/>
-      <c r="H73" s="3"/>
+      <c r="H73" s="22"/>
       <c r="I73" s="22"/>
       <c r="J73" s="15"/>
       <c r="L73" s="13" t="s">
@@ -3064,7 +3064,7 @@
       <c r="F78" s="22"/>
       <c r="G78" s="22"/>
       <c r="H78" s="22"/>
-      <c r="I78" s="15"/>
+      <c r="I78" s="22"/>
       <c r="J78" s="15"/>
       <c r="L78" s="13" t="s">
         <v>87</v>
@@ -3087,7 +3087,7 @@
       <c r="F79" s="22"/>
       <c r="G79" s="22"/>
       <c r="H79" s="22"/>
-      <c r="I79" s="15"/>
+      <c r="I79" s="22"/>
       <c r="J79" s="15"/>
       <c r="L79" s="13" t="s">
         <v>176</v>
@@ -3109,7 +3109,7 @@
       <c r="E80" s="22"/>
       <c r="F80" s="22"/>
       <c r="G80" s="22"/>
-      <c r="H80" s="3"/>
+      <c r="H80" s="22"/>
       <c r="I80" s="15"/>
       <c r="J80" s="15"/>
       <c r="L80" s="13" t="s">
@@ -3226,7 +3226,7 @@
       <c r="E85" s="22"/>
       <c r="F85" s="22"/>
       <c r="G85" s="22"/>
-      <c r="H85" s="3"/>
+      <c r="H85" s="22"/>
       <c r="I85" s="15"/>
       <c r="J85" s="15"/>
       <c r="L85" s="13" t="s">

</xml_diff>

<commit_message>
05.18 new files added
</commit_message>
<xml_diff>
--- a/Gyerekek.xlsx
+++ b/Gyerekek.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Privat\Informatika\Github\ZitaTuroczi1.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F5A7D2-1870-4F33-9CCE-872B4E9BB744}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7889779D-65C1-477E-AF3A-593FAF3E11EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18810" yWindow="555" windowWidth="9045" windowHeight="14880" xr2:uid="{D8DA68CD-37D4-4C3C-BD5C-8E37EBBBD311}"/>
   </bookViews>
@@ -1389,8 +1389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9286C3FF-60BE-42C4-89D5-9ACF7C2ACF54}">
   <dimension ref="A2:O96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1493,7 +1493,7 @@
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
       <c r="F5" s="22"/>
-      <c r="G5" s="15"/>
+      <c r="G5" s="22"/>
       <c r="H5" s="22"/>
       <c r="I5" s="32"/>
       <c r="J5" s="32"/>
@@ -1590,7 +1590,7 @@
       <c r="E9" s="22"/>
       <c r="F9" s="22"/>
       <c r="G9" s="22"/>
-      <c r="H9" s="15"/>
+      <c r="H9" s="22"/>
       <c r="I9" s="32"/>
       <c r="J9" s="32"/>
       <c r="L9" s="13" t="s">
@@ -1615,7 +1615,7 @@
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
       <c r="G10" s="22"/>
-      <c r="H10" s="3"/>
+      <c r="H10" s="22"/>
       <c r="I10" s="32"/>
       <c r="J10" s="32"/>
       <c r="L10" s="13" t="s">
@@ -1773,7 +1773,7 @@
       <c r="E18" s="22"/>
       <c r="F18" s="22"/>
       <c r="G18" s="22"/>
-      <c r="H18" s="15"/>
+      <c r="H18" s="22"/>
       <c r="I18" s="32"/>
       <c r="J18" s="32"/>
       <c r="L18" s="13" t="s">
@@ -1798,7 +1798,7 @@
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
       <c r="G19" s="22"/>
-      <c r="H19" s="15"/>
+      <c r="H19" s="22"/>
       <c r="I19" s="32"/>
       <c r="J19" s="32"/>
       <c r="L19" s="13" t="s">
@@ -2023,7 +2023,7 @@
       </c>
       <c r="C29" s="25"/>
       <c r="D29" s="22"/>
-      <c r="E29" s="3"/>
+      <c r="E29" s="22"/>
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
       <c r="H29" s="3"/>
@@ -2999,7 +2999,7 @@
       <c r="F75" s="22"/>
       <c r="G75" s="22"/>
       <c r="H75" s="22"/>
-      <c r="I75" s="15"/>
+      <c r="I75" s="22"/>
       <c r="J75" s="15"/>
       <c r="L75" s="13" t="s">
         <v>173</v>
@@ -3110,7 +3110,7 @@
       <c r="F80" s="22"/>
       <c r="G80" s="22"/>
       <c r="H80" s="22"/>
-      <c r="I80" s="15"/>
+      <c r="I80" s="22"/>
       <c r="J80" s="15"/>
       <c r="L80" s="13" t="s">
         <v>178</v>
@@ -3133,7 +3133,7 @@
       <c r="F81" s="22"/>
       <c r="G81" s="22"/>
       <c r="H81" s="22"/>
-      <c r="I81" s="15"/>
+      <c r="I81" s="22"/>
       <c r="J81" s="15"/>
       <c r="L81" s="13" t="s">
         <v>180</v>
@@ -3156,7 +3156,7 @@
       <c r="F82" s="22"/>
       <c r="G82" s="22"/>
       <c r="H82" s="3"/>
-      <c r="I82" s="15"/>
+      <c r="I82" s="22"/>
       <c r="J82" s="15"/>
       <c r="L82" s="13" t="s">
         <v>182</v>
@@ -3369,7 +3369,7 @@
       <c r="C93" s="25"/>
       <c r="D93" s="22"/>
       <c r="E93" s="22"/>
-      <c r="F93" s="15"/>
+      <c r="F93" s="22"/>
       <c r="G93" s="42"/>
       <c r="H93" s="32"/>
       <c r="I93" s="32"/>

</xml_diff>

<commit_message>
05.20 new files added plus A5 kepkeret feladat
</commit_message>
<xml_diff>
--- a/Gyerekek.xlsx
+++ b/Gyerekek.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Privat\Informatika\Github\ZitaTuroczi1.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7889779D-65C1-477E-AF3A-593FAF3E11EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E91B64-8465-424B-8DDA-F7DADBB66B30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18810" yWindow="555" windowWidth="9045" windowHeight="14880" xr2:uid="{D8DA68CD-37D4-4C3C-BD5C-8E37EBBBD311}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="228">
   <si>
     <t xml:space="preserve">Előképző 
 </t>
@@ -713,6 +713,9 @@
   </si>
   <si>
     <t>Zokni baba</t>
+  </si>
+  <si>
+    <t>Kép és kerete</t>
   </si>
 </sst>
 </file>
@@ -761,7 +764,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -972,21 +975,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
@@ -1065,13 +1059,6 @@
       <alignment textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hivatkozás" xfId="1" builtinId="8"/>
@@ -1389,8 +1376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9286C3FF-60BE-42C4-89D5-9ACF7C2ACF54}">
   <dimension ref="A2:O96"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K56" sqref="K56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2467,7 +2454,7 @@
       <c r="F50" s="22"/>
       <c r="G50" s="22"/>
       <c r="H50" s="15"/>
-      <c r="I50" s="15"/>
+      <c r="I50" s="22"/>
       <c r="J50" s="15"/>
       <c r="L50" s="13" t="s">
         <v>116</v>
@@ -2512,7 +2499,7 @@
       <c r="E52" s="15"/>
       <c r="F52" s="22"/>
       <c r="G52" s="15"/>
-      <c r="H52" s="15"/>
+      <c r="H52" s="22"/>
       <c r="I52" s="15"/>
       <c r="J52" s="15"/>
       <c r="L52" s="13" t="s">
@@ -3022,7 +3009,7 @@
       <c r="F76" s="22"/>
       <c r="G76" s="22"/>
       <c r="H76" s="22"/>
-      <c r="I76" s="15"/>
+      <c r="I76" s="22"/>
       <c r="J76" s="15"/>
       <c r="L76" s="13" t="s">
         <v>85</v>
@@ -3202,7 +3189,7 @@
       <c r="F84" s="22"/>
       <c r="G84" s="22"/>
       <c r="H84" s="22"/>
-      <c r="I84" s="15"/>
+      <c r="I84" s="22"/>
       <c r="J84" s="15"/>
       <c r="L84" s="13" t="s">
         <v>186</v>
@@ -3255,7 +3242,9 @@
       <c r="F88" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="G88" s="40"/>
+      <c r="G88" s="2" t="s">
+        <v>227</v>
+      </c>
       <c r="H88" s="37"/>
       <c r="I88" s="33"/>
       <c r="J88" s="33"/>
@@ -3281,7 +3270,9 @@
       <c r="F89" s="8">
         <v>43963</v>
       </c>
-      <c r="G89" s="41"/>
+      <c r="G89" s="8">
+        <v>43971</v>
+      </c>
       <c r="H89" s="38"/>
       <c r="I89" s="34"/>
       <c r="J89" s="34"/>
@@ -3301,7 +3292,7 @@
       <c r="D90" s="20"/>
       <c r="E90" s="20"/>
       <c r="F90" s="20"/>
-      <c r="G90" s="42"/>
+      <c r="G90" s="20"/>
       <c r="H90" s="32"/>
       <c r="I90" s="32"/>
       <c r="J90" s="32"/>
@@ -3323,8 +3314,8 @@
       <c r="C91" s="25"/>
       <c r="D91" s="22"/>
       <c r="E91" s="22"/>
-      <c r="F91" s="15"/>
-      <c r="G91" s="42"/>
+      <c r="F91" s="22"/>
+      <c r="G91" s="15"/>
       <c r="H91" s="32"/>
       <c r="I91" s="32"/>
       <c r="J91" s="32"/>
@@ -3347,7 +3338,7 @@
       <c r="D92" s="15"/>
       <c r="E92" s="15"/>
       <c r="F92" s="15"/>
-      <c r="G92" s="42"/>
+      <c r="G92" s="15"/>
       <c r="H92" s="32"/>
       <c r="I92" s="32"/>
       <c r="J92" s="32"/>
@@ -3370,7 +3361,7 @@
       <c r="D93" s="22"/>
       <c r="E93" s="22"/>
       <c r="F93" s="22"/>
-      <c r="G93" s="42"/>
+      <c r="G93" s="15"/>
       <c r="H93" s="32"/>
       <c r="I93" s="32"/>
       <c r="J93" s="32"/>
@@ -3394,8 +3385,8 @@
       <c r="C94" s="25"/>
       <c r="D94" s="22"/>
       <c r="E94" s="22"/>
-      <c r="F94" s="15"/>
-      <c r="G94" s="42"/>
+      <c r="F94" s="22"/>
+      <c r="G94" s="15"/>
       <c r="H94" s="32"/>
       <c r="I94" s="32"/>
       <c r="J94" s="32"/>
@@ -3416,8 +3407,8 @@
       <c r="C95" s="25"/>
       <c r="D95" s="22"/>
       <c r="E95" s="22"/>
-      <c r="F95" s="15"/>
-      <c r="G95" s="42"/>
+      <c r="F95" s="22"/>
+      <c r="G95" s="15"/>
       <c r="H95" s="32"/>
       <c r="I95" s="32"/>
       <c r="J95" s="32"/>

</xml_diff>

<commit_message>
05.21 new files + mecses
</commit_message>
<xml_diff>
--- a/Gyerekek.xlsx
+++ b/Gyerekek.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Privat\Informatika\Github\ZitaTuroczi1.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E91B64-8465-424B-8DDA-F7DADBB66B30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B283557-D724-43BA-9399-41B6695CAFBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18810" yWindow="555" windowWidth="9045" windowHeight="14880" xr2:uid="{D8DA68CD-37D4-4C3C-BD5C-8E37EBBBD311}"/>
+    <workbookView xWindow="13230" yWindow="795" windowWidth="12690" windowHeight="14880" xr2:uid="{D8DA68CD-37D4-4C3C-BD5C-8E37EBBBD311}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="229">
   <si>
     <t xml:space="preserve">Előképző 
 </t>
@@ -716,6 +716,9 @@
   </si>
   <si>
     <t>Kép és kerete</t>
+  </si>
+  <si>
+    <t>Mécsestartó</t>
   </si>
 </sst>
 </file>
@@ -1374,10 +1377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9286C3FF-60BE-42C4-89D5-9ACF7C2ACF54}">
-  <dimension ref="A2:O96"/>
+  <dimension ref="A2:P96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K56" sqref="K56"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N70" sqref="N70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1386,13 +1389,14 @@
     <col min="2" max="2" width="26.7109375" style="31" bestFit="1" customWidth="1"/>
     <col min="3" max="8" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="3.7109375" style="31" customWidth="1"/>
-    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12" customWidth="1"/>
-    <col min="14" max="14" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.140625" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12" customWidth="1"/>
+    <col min="15" max="15" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" s="1" customFormat="1" ht="101.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" s="1" customFormat="1" ht="101.25" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
@@ -1420,7 +1424,7 @@
       <c r="I2" s="33"/>
       <c r="J2" s="33"/>
     </row>
-    <row r="3" spans="1:14" s="1" customFormat="1" ht="42" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" s="1" customFormat="1" ht="42" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
       <c r="B3" s="28">
         <v>2020</v>
@@ -1446,7 +1450,7 @@
       <c r="I3" s="34"/>
       <c r="J3" s="34"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>1</v>
       </c>
@@ -1461,15 +1465,15 @@
       <c r="H4" s="20"/>
       <c r="I4" s="32"/>
       <c r="J4" s="32"/>
-      <c r="L4" s="13" t="s">
+      <c r="M4" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="M4" s="13"/>
-      <c r="N4" s="14" t="s">
+      <c r="N4" s="13"/>
+      <c r="O4" s="14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>2</v>
       </c>
@@ -1484,17 +1488,17 @@
       <c r="H5" s="22"/>
       <c r="I5" s="32"/>
       <c r="J5" s="32"/>
-      <c r="L5" s="13" t="s">
+      <c r="M5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="13" t="s">
+      <c r="N5" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="N5" s="14" t="s">
+      <c r="O5" s="14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>3</v>
       </c>
@@ -1506,20 +1510,20 @@
       <c r="E6" s="22"/>
       <c r="F6" s="22"/>
       <c r="G6" s="22"/>
-      <c r="H6" s="15"/>
+      <c r="H6" s="22"/>
       <c r="I6" s="32"/>
       <c r="J6" s="32"/>
-      <c r="L6" s="13" t="s">
+      <c r="M6" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="M6" s="13" t="s">
+      <c r="N6" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="N6" s="14" t="s">
+      <c r="O6" s="14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>4</v>
       </c>
@@ -1534,15 +1538,15 @@
       <c r="H7" s="15"/>
       <c r="I7" s="32"/>
       <c r="J7" s="32"/>
-      <c r="L7" s="13" t="s">
+      <c r="M7" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="M7" s="13"/>
-      <c r="N7" s="14" t="s">
+      <c r="N7" s="13"/>
+      <c r="O7" s="14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>5</v>
       </c>
@@ -1557,15 +1561,15 @@
       <c r="H8" s="15"/>
       <c r="I8" s="32"/>
       <c r="J8" s="32"/>
-      <c r="L8" s="13" t="s">
+      <c r="M8" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="M8" s="13"/>
-      <c r="N8" s="14" t="s">
+      <c r="N8" s="13"/>
+      <c r="O8" s="14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>6</v>
       </c>
@@ -1580,17 +1584,17 @@
       <c r="H9" s="22"/>
       <c r="I9" s="32"/>
       <c r="J9" s="32"/>
-      <c r="L9" s="13" t="s">
+      <c r="M9" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="M9" s="13" t="s">
+      <c r="N9" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="N9" s="14" t="s">
+      <c r="O9" s="14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>7</v>
       </c>
@@ -1605,17 +1609,17 @@
       <c r="H10" s="22"/>
       <c r="I10" s="32"/>
       <c r="J10" s="32"/>
-      <c r="L10" s="13" t="s">
+      <c r="M10" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="M10" s="13" t="s">
+      <c r="N10" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="N10" s="14" t="s">
+      <c r="O10" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>8</v>
       </c>
@@ -1625,20 +1629,20 @@
       <c r="C11" s="25"/>
       <c r="D11" s="22"/>
       <c r="E11" s="22"/>
-      <c r="F11" s="3"/>
+      <c r="F11" s="22"/>
       <c r="G11" s="22"/>
       <c r="H11" s="22"/>
       <c r="I11" s="32"/>
       <c r="J11" s="32"/>
-      <c r="L11" s="13" t="s">
+      <c r="M11" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="M11" s="13"/>
-      <c r="N11" s="14" t="s">
+      <c r="N11" s="13"/>
+      <c r="O11" s="14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>9</v>
       </c>
@@ -1653,17 +1657,17 @@
       <c r="H12" s="3"/>
       <c r="I12" s="32"/>
       <c r="J12" s="32"/>
-      <c r="L12" s="13" t="s">
+      <c r="M12" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="M12" s="13" t="s">
+      <c r="N12" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="N12" s="14" t="s">
+      <c r="O12" s="14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="101.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="101.25" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>0</v>
       </c>
@@ -1694,8 +1698,9 @@
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
-    </row>
-    <row r="16" spans="1:14" ht="42" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O15" s="1"/>
+    </row>
+    <row r="16" spans="1:15" ht="42" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10"/>
       <c r="B16" s="28">
         <v>2020</v>
@@ -1724,8 +1729,9 @@
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O16" s="1"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <v>1</v>
       </c>
@@ -1740,15 +1746,15 @@
       <c r="H17" s="20"/>
       <c r="I17" s="32"/>
       <c r="J17" s="32"/>
-      <c r="L17" s="13" t="s">
+      <c r="M17" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="M17" s="13"/>
-      <c r="N17" s="14" t="s">
+      <c r="N17" s="13"/>
+      <c r="O17" s="14" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>2</v>
       </c>
@@ -1763,17 +1769,17 @@
       <c r="H18" s="22"/>
       <c r="I18" s="32"/>
       <c r="J18" s="32"/>
-      <c r="L18" s="13" t="s">
+      <c r="M18" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="M18" s="13" t="s">
+      <c r="N18" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="N18" s="14" t="s">
+      <c r="O18" s="14" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>3</v>
       </c>
@@ -1788,17 +1794,17 @@
       <c r="H19" s="22"/>
       <c r="I19" s="32"/>
       <c r="J19" s="32"/>
-      <c r="L19" s="13" t="s">
+      <c r="M19" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="M19" s="13" t="s">
+      <c r="N19" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="N19" s="14" t="s">
+      <c r="O19" s="14" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>4</v>
       </c>
@@ -1813,15 +1819,15 @@
       <c r="H20" s="15"/>
       <c r="I20" s="32"/>
       <c r="J20" s="32"/>
-      <c r="L20" s="13" t="s">
+      <c r="M20" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="M20" s="13"/>
-      <c r="N20" s="14" t="s">
+      <c r="N20" s="13"/>
+      <c r="O20" s="14" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>5</v>
       </c>
@@ -1836,15 +1842,15 @@
       <c r="H21" s="22"/>
       <c r="I21" s="32"/>
       <c r="J21" s="32"/>
-      <c r="L21" s="13" t="s">
+      <c r="M21" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="M21" s="13"/>
-      <c r="N21" s="14" t="s">
+      <c r="N21" s="13"/>
+      <c r="O21" s="14" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>6</v>
       </c>
@@ -1859,15 +1865,15 @@
       <c r="H22" s="15"/>
       <c r="I22" s="32"/>
       <c r="J22" s="32"/>
-      <c r="L22" s="13" t="s">
+      <c r="M22" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="M22" s="13"/>
-      <c r="N22" s="14" t="s">
+      <c r="N22" s="13"/>
+      <c r="O22" s="14" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <v>7</v>
       </c>
@@ -1882,15 +1888,15 @@
       <c r="H23" s="15"/>
       <c r="I23" s="32"/>
       <c r="J23" s="32"/>
-      <c r="L23" s="13" t="s">
+      <c r="M23" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="M23" s="13"/>
-      <c r="N23" s="14" t="s">
+      <c r="N23" s="13"/>
+      <c r="O23" s="14" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="16">
         <v>8</v>
       </c>
@@ -1905,15 +1911,15 @@
       <c r="H24" s="22"/>
       <c r="I24" s="32"/>
       <c r="J24" s="32"/>
-      <c r="L24" s="13" t="s">
+      <c r="M24" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="M24" s="13"/>
-      <c r="N24" s="14" t="s">
+      <c r="N24" s="13"/>
+      <c r="O24" s="14" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="16">
         <v>9</v>
       </c>
@@ -1928,15 +1934,15 @@
       <c r="H25" s="22"/>
       <c r="I25" s="32"/>
       <c r="J25" s="32"/>
-      <c r="L25" s="13" t="s">
+      <c r="M25" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="M25" s="13"/>
-      <c r="N25" s="14" t="s">
+      <c r="N25" s="13"/>
+      <c r="O25" s="14" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="17">
         <v>10</v>
       </c>
@@ -1951,13 +1957,13 @@
       <c r="H26" s="22"/>
       <c r="I26" s="32"/>
       <c r="J26" s="32"/>
-      <c r="L26" s="13" t="s">
+      <c r="M26" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="M26" s="13"/>
-      <c r="N26" s="14"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N26" s="13"/>
+      <c r="O26" s="14"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="17">
         <v>11</v>
       </c>
@@ -1972,17 +1978,17 @@
       <c r="H27" s="22"/>
       <c r="I27" s="32"/>
       <c r="J27" s="32"/>
-      <c r="L27" s="13" t="s">
+      <c r="M27" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="M27" s="13" t="s">
+      <c r="N27" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="N27" s="14" t="s">
+      <c r="O27" s="14" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="17">
         <v>12</v>
       </c>
@@ -1997,11 +2003,11 @@
       <c r="H28" s="22"/>
       <c r="I28" s="32"/>
       <c r="J28" s="32"/>
-      <c r="L28" s="13"/>
       <c r="M28" s="13"/>
-      <c r="N28" s="14"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N28" s="13"/>
+      <c r="O28" s="14"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="17">
         <v>13</v>
       </c>
@@ -2016,15 +2022,15 @@
       <c r="H29" s="3"/>
       <c r="I29" s="32"/>
       <c r="J29" s="32"/>
-      <c r="L29" s="13" t="s">
+      <c r="M29" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="M29" s="13"/>
-      <c r="N29" s="14" t="s">
+      <c r="N29" s="13"/>
+      <c r="O29" s="14" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="101.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" ht="101.25" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>0</v>
       </c>
@@ -2055,8 +2061,9 @@
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
-    </row>
-    <row r="33" spans="1:15" ht="42" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O32" s="1"/>
+    </row>
+    <row r="33" spans="1:16" ht="42" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="10"/>
       <c r="B33" s="28">
         <v>2020</v>
@@ -2085,8 +2092,9 @@
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O33" s="1"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="11">
         <v>1</v>
       </c>
@@ -2101,20 +2109,20 @@
       <c r="H34" s="23"/>
       <c r="I34" s="32"/>
       <c r="J34" s="32"/>
-      <c r="L34" s="13" t="s">
+      <c r="M34" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="M34" s="13" t="s">
+      <c r="N34" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="N34" s="14" t="s">
+      <c r="O34" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="O34" s="14" t="s">
+      <c r="P34" s="14" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <v>2</v>
       </c>
@@ -2129,15 +2137,15 @@
       <c r="H35" s="22"/>
       <c r="I35" s="32"/>
       <c r="J35" s="32"/>
-      <c r="L35" s="13" t="s">
+      <c r="M35" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="M35" s="13"/>
-      <c r="N35" s="14" t="s">
+      <c r="N35" s="13"/>
+      <c r="O35" s="14" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
         <v>3</v>
       </c>
@@ -2152,15 +2160,15 @@
       <c r="H36" s="22"/>
       <c r="I36" s="32"/>
       <c r="J36" s="32"/>
-      <c r="L36" s="13" t="s">
+      <c r="M36" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="M36" s="13"/>
-      <c r="N36" s="14" t="s">
+      <c r="N36" s="13"/>
+      <c r="O36" s="14" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
         <v>4</v>
       </c>
@@ -2175,15 +2183,15 @@
       <c r="H37" s="22"/>
       <c r="I37" s="32"/>
       <c r="J37" s="32"/>
-      <c r="L37" s="13" t="s">
+      <c r="M37" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="M37" s="13"/>
-      <c r="N37" s="14" t="s">
+      <c r="N37" s="13"/>
+      <c r="O37" s="14" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
         <v>5</v>
       </c>
@@ -2198,15 +2206,15 @@
       <c r="H38" s="15"/>
       <c r="I38" s="32"/>
       <c r="J38" s="32"/>
-      <c r="L38" s="13" t="s">
+      <c r="M38" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="M38" s="13"/>
-      <c r="N38" s="14" t="s">
+      <c r="N38" s="13"/>
+      <c r="O38" s="14" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
         <v>6</v>
       </c>
@@ -2221,15 +2229,15 @@
       <c r="H39" s="22"/>
       <c r="I39" s="32"/>
       <c r="J39" s="32"/>
-      <c r="L39" s="13" t="s">
+      <c r="M39" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="M39" s="13"/>
-      <c r="N39" s="14" t="s">
+      <c r="N39" s="13"/>
+      <c r="O39" s="14" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
         <v>7</v>
       </c>
@@ -2244,17 +2252,17 @@
       <c r="H40" s="15"/>
       <c r="I40" s="32"/>
       <c r="J40" s="32"/>
-      <c r="L40" s="13" t="s">
+      <c r="M40" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="M40" s="13" t="s">
+      <c r="N40" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="N40" s="14" t="s">
+      <c r="O40" s="14" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="16">
         <v>8</v>
       </c>
@@ -2269,15 +2277,15 @@
       <c r="H41" s="15"/>
       <c r="I41" s="32"/>
       <c r="J41" s="32"/>
-      <c r="L41" s="13" t="s">
+      <c r="M41" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="M41" s="13"/>
-      <c r="N41" s="14" t="s">
+      <c r="N41" s="13"/>
+      <c r="O41" s="14" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="99" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" ht="99" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>122</v>
       </c>
@@ -2308,12 +2316,15 @@
       <c r="J44" s="35" t="s">
         <v>226</v>
       </c>
-      <c r="K44" s="1"/>
+      <c r="K44" s="35" t="s">
+        <v>228</v>
+      </c>
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
       <c r="N44" s="1"/>
-    </row>
-    <row r="45" spans="1:15" ht="42" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O44" s="1"/>
+    </row>
+    <row r="45" spans="1:16" ht="42" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="10"/>
       <c r="B45" s="28">
         <v>2020</v>
@@ -2342,12 +2353,15 @@
       <c r="J45" s="36">
         <v>43965</v>
       </c>
-      <c r="K45" s="1"/>
+      <c r="K45" s="36">
+        <v>43972</v>
+      </c>
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O45" s="1"/>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="11">
         <v>1</v>
       </c>
@@ -2362,15 +2376,16 @@
       <c r="H46" s="20"/>
       <c r="I46" s="20"/>
       <c r="J46" s="20"/>
-      <c r="L46" s="13" t="s">
+      <c r="K46" s="20"/>
+      <c r="M46" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="M46" s="13"/>
-      <c r="N46" s="14" t="s">
+      <c r="N46" s="13"/>
+      <c r="O46" s="14" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="12">
         <v>2</v>
       </c>
@@ -2385,15 +2400,16 @@
       <c r="H47" s="15"/>
       <c r="I47" s="15"/>
       <c r="J47" s="15"/>
-      <c r="L47" s="13" t="s">
+      <c r="K47" s="15"/>
+      <c r="M47" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="M47" s="13"/>
-      <c r="N47" s="14" t="s">
+      <c r="N47" s="13"/>
+      <c r="O47" s="14" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="12">
         <v>3</v>
       </c>
@@ -2408,17 +2424,18 @@
       <c r="H48" s="22"/>
       <c r="I48" s="15"/>
       <c r="J48" s="15"/>
-      <c r="L48" s="13" t="s">
+      <c r="K48" s="15"/>
+      <c r="M48" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="M48" s="13" t="s">
+      <c r="N48" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="N48" s="14" t="s">
+      <c r="O48" s="14" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="12">
         <v>4</v>
       </c>
@@ -2433,15 +2450,16 @@
       <c r="H49" s="15"/>
       <c r="I49" s="15"/>
       <c r="J49" s="15"/>
-      <c r="L49" s="13" t="s">
+      <c r="K49" s="15"/>
+      <c r="M49" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="M49" s="13"/>
-      <c r="N49" s="14" t="s">
+      <c r="N49" s="13"/>
+      <c r="O49" s="14" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="12">
         <v>5</v>
       </c>
@@ -2456,15 +2474,16 @@
       <c r="H50" s="15"/>
       <c r="I50" s="22"/>
       <c r="J50" s="15"/>
-      <c r="L50" s="13" t="s">
+      <c r="K50" s="15"/>
+      <c r="M50" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="M50" s="13"/>
-      <c r="N50" s="14" t="s">
+      <c r="N50" s="13"/>
+      <c r="O50" s="14" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="12">
         <v>6</v>
       </c>
@@ -2479,15 +2498,16 @@
       <c r="H51" s="15"/>
       <c r="I51" s="15"/>
       <c r="J51" s="15"/>
-      <c r="L51" s="13" t="s">
+      <c r="K51" s="15"/>
+      <c r="M51" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="M51" s="13"/>
-      <c r="N51" s="14" t="s">
+      <c r="N51" s="13"/>
+      <c r="O51" s="14" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="12">
         <v>7</v>
       </c>
@@ -2502,15 +2522,16 @@
       <c r="H52" s="22"/>
       <c r="I52" s="15"/>
       <c r="J52" s="15"/>
-      <c r="L52" s="13" t="s">
+      <c r="K52" s="15"/>
+      <c r="M52" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="M52" s="13"/>
-      <c r="N52" s="14" t="s">
+      <c r="N52" s="13"/>
+      <c r="O52" s="14" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="99" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" ht="99" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>122</v>
       </c>
@@ -2541,12 +2562,15 @@
       <c r="J55" s="35" t="s">
         <v>226</v>
       </c>
-      <c r="K55" s="1"/>
+      <c r="K55" s="35" t="s">
+        <v>228</v>
+      </c>
       <c r="L55" s="1"/>
       <c r="M55" s="1"/>
       <c r="N55" s="1"/>
-    </row>
-    <row r="56" spans="1:14" ht="42" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O55" s="1"/>
+    </row>
+    <row r="56" spans="1:15" ht="42" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="10"/>
       <c r="B56" s="28">
         <v>2020</v>
@@ -2575,12 +2599,15 @@
       <c r="J56" s="36">
         <v>43965</v>
       </c>
-      <c r="K56" s="1"/>
+      <c r="K56" s="36">
+        <v>43972</v>
+      </c>
       <c r="L56" s="1"/>
       <c r="M56" s="1"/>
       <c r="N56" s="1"/>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O56" s="1"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
         <v>1</v>
       </c>
@@ -2595,15 +2622,16 @@
       <c r="H57" s="20"/>
       <c r="I57" s="20"/>
       <c r="J57" s="20"/>
-      <c r="L57" s="13" t="s">
+      <c r="K57" s="20"/>
+      <c r="M57" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="M57" s="13"/>
-      <c r="N57" s="14" t="s">
+      <c r="N57" s="13"/>
+      <c r="O57" s="14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="12">
         <v>2</v>
       </c>
@@ -2618,15 +2646,16 @@
       <c r="H58" s="22"/>
       <c r="I58" s="22"/>
       <c r="J58" s="22"/>
-      <c r="L58" s="13" t="s">
+      <c r="K58" s="15"/>
+      <c r="M58" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="M58" s="13"/>
-      <c r="N58" s="14" t="s">
+      <c r="N58" s="13"/>
+      <c r="O58" s="14" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="12">
         <v>3</v>
       </c>
@@ -2641,15 +2670,16 @@
       <c r="H59" s="15"/>
       <c r="I59" s="22"/>
       <c r="J59" s="15"/>
-      <c r="L59" s="13" t="s">
+      <c r="K59" s="15"/>
+      <c r="M59" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="M59" s="13"/>
-      <c r="N59" s="14" t="s">
+      <c r="N59" s="13"/>
+      <c r="O59" s="14" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="12">
         <v>4</v>
       </c>
@@ -2664,15 +2694,16 @@
       <c r="H60" s="15"/>
       <c r="I60" s="15"/>
       <c r="J60" s="15"/>
-      <c r="L60" s="13" t="s">
+      <c r="K60" s="15"/>
+      <c r="M60" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="M60" s="13"/>
-      <c r="N60" s="14" t="s">
+      <c r="N60" s="13"/>
+      <c r="O60" s="14" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="12">
         <v>5</v>
       </c>
@@ -2687,17 +2718,18 @@
       <c r="H61" s="15"/>
       <c r="I61" s="15"/>
       <c r="J61" s="15"/>
-      <c r="L61" s="13" t="s">
+      <c r="K61" s="15"/>
+      <c r="M61" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="M61" s="13" t="s">
+      <c r="N61" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="N61" s="14" t="s">
+      <c r="O61" s="14" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" s="12">
         <v>6</v>
       </c>
@@ -2711,16 +2743,17 @@
       <c r="G62" s="22"/>
       <c r="H62" s="22"/>
       <c r="I62" s="22"/>
-      <c r="J62" s="15"/>
-      <c r="L62" s="13" t="s">
+      <c r="J62" s="22"/>
+      <c r="K62" s="15"/>
+      <c r="M62" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="M62" s="13"/>
-      <c r="N62" s="14" t="s">
+      <c r="N62" s="13"/>
+      <c r="O62" s="14" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="12">
         <v>7</v>
       </c>
@@ -2735,15 +2768,16 @@
       <c r="H63" s="22"/>
       <c r="I63" s="22"/>
       <c r="J63" s="22"/>
-      <c r="L63" s="13" t="s">
+      <c r="K63" s="15"/>
+      <c r="M63" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="M63" s="13"/>
-      <c r="N63" s="14" t="s">
+      <c r="N63" s="13"/>
+      <c r="O63" s="14" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="16">
         <v>8</v>
       </c>
@@ -2758,15 +2792,16 @@
       <c r="H64" s="22"/>
       <c r="I64" s="22"/>
       <c r="J64" s="15"/>
-      <c r="L64" s="13" t="s">
+      <c r="K64" s="15"/>
+      <c r="M64" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="M64" s="13"/>
-      <c r="N64" s="14" t="s">
+      <c r="N64" s="13"/>
+      <c r="O64" s="14" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="16">
         <v>9</v>
       </c>
@@ -2781,15 +2816,16 @@
       <c r="H65" s="22"/>
       <c r="I65" s="22"/>
       <c r="J65" s="15"/>
-      <c r="L65" s="13" t="s">
+      <c r="K65" s="15"/>
+      <c r="M65" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="M65" s="13"/>
-      <c r="N65" s="14" t="s">
+      <c r="N65" s="13"/>
+      <c r="O65" s="14" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" s="17">
         <v>10</v>
       </c>
@@ -2802,15 +2838,16 @@
       <c r="F66" s="15"/>
       <c r="G66" s="15"/>
       <c r="H66" s="22"/>
-      <c r="I66" s="15"/>
+      <c r="I66" s="22"/>
       <c r="J66" s="15"/>
-      <c r="L66" s="13" t="s">
+      <c r="K66" s="15"/>
+      <c r="M66" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="M66" s="13"/>
-      <c r="N66" s="14"/>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N66" s="13"/>
+      <c r="O66" s="14"/>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" s="17">
         <v>11</v>
       </c>
@@ -2825,15 +2862,16 @@
       <c r="H67" s="22"/>
       <c r="I67" s="22"/>
       <c r="J67" s="15"/>
-      <c r="L67" s="13" t="s">
+      <c r="K67" s="15"/>
+      <c r="M67" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="M67" s="13"/>
-      <c r="N67" s="14" t="s">
+      <c r="N67" s="13"/>
+      <c r="O67" s="14" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="99" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" ht="99" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
         <v>122</v>
       </c>
@@ -2864,12 +2902,15 @@
       <c r="J70" s="35" t="s">
         <v>226</v>
       </c>
-      <c r="K70" s="1"/>
+      <c r="K70" s="35" t="s">
+        <v>228</v>
+      </c>
       <c r="L70" s="1"/>
       <c r="M70" s="1"/>
       <c r="N70" s="1"/>
-    </row>
-    <row r="71" spans="1:14" ht="42" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O70" s="1"/>
+    </row>
+    <row r="71" spans="1:15" ht="42" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="10"/>
       <c r="B71" s="28">
         <v>2020</v>
@@ -2898,12 +2939,15 @@
       <c r="J71" s="36">
         <v>43965</v>
       </c>
-      <c r="K71" s="1"/>
+      <c r="K71" s="36">
+        <v>43972</v>
+      </c>
       <c r="L71" s="1"/>
       <c r="M71" s="1"/>
       <c r="N71" s="1"/>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O71" s="1"/>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" s="11">
         <v>1</v>
       </c>
@@ -2918,17 +2962,18 @@
       <c r="H72" s="4"/>
       <c r="I72" s="20"/>
       <c r="J72" s="20"/>
-      <c r="L72" s="13" t="s">
+      <c r="K72" s="20"/>
+      <c r="M72" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="M72" s="13" t="s">
+      <c r="N72" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="N72" s="14" t="s">
+      <c r="O72" s="14" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" s="17">
         <v>2</v>
       </c>
@@ -2943,14 +2988,15 @@
       <c r="H73" s="22"/>
       <c r="I73" s="22"/>
       <c r="J73" s="15"/>
-      <c r="L73" s="13" t="s">
+      <c r="K73" s="15"/>
+      <c r="M73" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="N73" s="14" t="s">
+      <c r="O73" s="14" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" s="12">
         <v>3</v>
       </c>
@@ -2965,15 +3011,16 @@
       <c r="H74" s="3"/>
       <c r="I74" s="15"/>
       <c r="J74" s="15"/>
-      <c r="L74" s="13" t="s">
+      <c r="K74" s="15"/>
+      <c r="M74" s="13" t="s">
         <v>171</v>
       </c>
-      <c r="M74" s="13"/>
-      <c r="N74" s="14" t="s">
+      <c r="N74" s="13"/>
+      <c r="O74" s="14" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" s="12">
         <v>4</v>
       </c>
@@ -2988,15 +3035,16 @@
       <c r="H75" s="22"/>
       <c r="I75" s="22"/>
       <c r="J75" s="15"/>
-      <c r="L75" s="13" t="s">
+      <c r="K75" s="15"/>
+      <c r="M75" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="M75" s="13"/>
-      <c r="N75" s="14" t="s">
+      <c r="N75" s="13"/>
+      <c r="O75" s="14" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" s="12">
         <v>5</v>
       </c>
@@ -3011,15 +3059,16 @@
       <c r="H76" s="22"/>
       <c r="I76" s="22"/>
       <c r="J76" s="15"/>
-      <c r="L76" s="13" t="s">
+      <c r="K76" s="15"/>
+      <c r="M76" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="M76" s="13"/>
-      <c r="N76" s="14" t="s">
+      <c r="N76" s="13"/>
+      <c r="O76" s="14" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" s="12">
         <v>6</v>
       </c>
@@ -3034,11 +3083,12 @@
       <c r="H77" s="3"/>
       <c r="I77" s="15"/>
       <c r="J77" s="15"/>
-      <c r="L77" s="13"/>
+      <c r="K77" s="15"/>
       <c r="M77" s="13"/>
-      <c r="N77" s="14"/>
-    </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N77" s="13"/>
+      <c r="O77" s="14"/>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" s="12">
         <v>7</v>
       </c>
@@ -3053,15 +3103,16 @@
       <c r="H78" s="22"/>
       <c r="I78" s="22"/>
       <c r="J78" s="15"/>
-      <c r="L78" s="13" t="s">
+      <c r="K78" s="15"/>
+      <c r="M78" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="M78" s="13"/>
-      <c r="N78" s="14" t="s">
+      <c r="N78" s="13"/>
+      <c r="O78" s="14" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" s="12">
         <v>8</v>
       </c>
@@ -3076,15 +3127,16 @@
       <c r="H79" s="22"/>
       <c r="I79" s="22"/>
       <c r="J79" s="15"/>
-      <c r="L79" s="13" t="s">
+      <c r="K79" s="15"/>
+      <c r="M79" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="M79" s="13"/>
-      <c r="N79" s="14" t="s">
+      <c r="N79" s="13"/>
+      <c r="O79" s="14" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" s="16">
         <v>9</v>
       </c>
@@ -3099,15 +3151,16 @@
       <c r="H80" s="22"/>
       <c r="I80" s="22"/>
       <c r="J80" s="15"/>
-      <c r="L80" s="13" t="s">
+      <c r="K80" s="15"/>
+      <c r="M80" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="M80" s="13"/>
-      <c r="N80" s="14" t="s">
+      <c r="N80" s="13"/>
+      <c r="O80" s="14" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" s="16">
         <v>10</v>
       </c>
@@ -3122,15 +3175,16 @@
       <c r="H81" s="22"/>
       <c r="I81" s="22"/>
       <c r="J81" s="15"/>
-      <c r="L81" s="13" t="s">
+      <c r="K81" s="15"/>
+      <c r="M81" s="13" t="s">
         <v>180</v>
       </c>
-      <c r="M81" s="13"/>
-      <c r="N81" s="14" t="s">
+      <c r="N81" s="13"/>
+      <c r="O81" s="14" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" s="17">
         <v>11</v>
       </c>
@@ -3145,15 +3199,16 @@
       <c r="H82" s="3"/>
       <c r="I82" s="22"/>
       <c r="J82" s="15"/>
-      <c r="L82" s="13" t="s">
+      <c r="K82" s="15"/>
+      <c r="M82" s="13" t="s">
         <v>182</v>
       </c>
-      <c r="M82" s="13"/>
-      <c r="N82" s="14" t="s">
+      <c r="N82" s="13"/>
+      <c r="O82" s="14" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83" s="17">
         <v>12</v>
       </c>
@@ -3168,15 +3223,16 @@
       <c r="H83" s="3"/>
       <c r="I83" s="15"/>
       <c r="J83" s="15"/>
-      <c r="L83" s="13" t="s">
+      <c r="K83" s="15"/>
+      <c r="M83" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="M83" s="13"/>
-      <c r="N83" s="14" t="s">
+      <c r="N83" s="13"/>
+      <c r="O83" s="14" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" s="17">
         <v>13</v>
       </c>
@@ -3191,17 +3247,18 @@
       <c r="H84" s="22"/>
       <c r="I84" s="22"/>
       <c r="J84" s="15"/>
-      <c r="L84" s="13" t="s">
+      <c r="K84" s="15"/>
+      <c r="M84" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="M84" s="13" t="s">
+      <c r="N84" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="N84" s="14" t="s">
+      <c r="O84" s="14" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" s="17">
         <v>14</v>
       </c>
@@ -3216,14 +3273,15 @@
       <c r="H85" s="22"/>
       <c r="I85" s="15"/>
       <c r="J85" s="15"/>
-      <c r="L85" s="13" t="s">
+      <c r="K85" s="15"/>
+      <c r="M85" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="N85" s="14" t="s">
+      <c r="O85" s="14" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="88" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" ht="105" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
         <v>122</v>
       </c>
@@ -3252,8 +3310,9 @@
       <c r="L88" s="1"/>
       <c r="M88" s="1"/>
       <c r="N88" s="1"/>
-    </row>
-    <row r="89" spans="1:14" ht="42" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O88" s="1"/>
+    </row>
+    <row r="89" spans="1:15" ht="42" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="10"/>
       <c r="B89" s="28">
         <v>2020</v>
@@ -3280,8 +3339,9 @@
       <c r="L89" s="1"/>
       <c r="M89" s="1"/>
       <c r="N89" s="1"/>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O89" s="1"/>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" s="11">
         <v>1</v>
       </c>
@@ -3296,15 +3356,15 @@
       <c r="H90" s="32"/>
       <c r="I90" s="32"/>
       <c r="J90" s="32"/>
-      <c r="L90" s="13" t="s">
+      <c r="M90" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="M90" s="13"/>
-      <c r="N90" s="14" t="s">
+      <c r="N90" s="13"/>
+      <c r="O90" s="14" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" s="12">
         <v>2</v>
       </c>
@@ -3319,15 +3379,15 @@
       <c r="H91" s="32"/>
       <c r="I91" s="32"/>
       <c r="J91" s="32"/>
-      <c r="L91" s="13" t="s">
+      <c r="M91" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="M91" s="13"/>
-      <c r="N91" s="14" t="s">
+      <c r="N91" s="13"/>
+      <c r="O91" s="14" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" s="12">
         <v>3</v>
       </c>
@@ -3342,15 +3402,15 @@
       <c r="H92" s="32"/>
       <c r="I92" s="32"/>
       <c r="J92" s="32"/>
-      <c r="L92" s="13" t="s">
+      <c r="M92" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="M92" s="13"/>
-      <c r="N92" s="14" t="s">
+      <c r="N92" s="13"/>
+      <c r="O92" s="14" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" s="12">
         <v>4</v>
       </c>
@@ -3365,17 +3425,17 @@
       <c r="H93" s="32"/>
       <c r="I93" s="32"/>
       <c r="J93" s="32"/>
-      <c r="L93" s="13" t="s">
+      <c r="M93" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="M93" s="13" t="s">
+      <c r="N93" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="N93" s="14" t="s">
+      <c r="O93" s="14" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" s="12">
         <v>5</v>
       </c>
@@ -3390,14 +3450,14 @@
       <c r="H94" s="32"/>
       <c r="I94" s="32"/>
       <c r="J94" s="32"/>
-      <c r="L94" s="13" t="s">
+      <c r="M94" s="13" t="s">
         <v>205</v>
       </c>
-      <c r="N94" s="14" t="s">
+      <c r="O94" s="14" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95" s="12">
         <v>6</v>
       </c>
@@ -3412,86 +3472,86 @@
       <c r="H95" s="32"/>
       <c r="I95" s="32"/>
       <c r="J95" s="32"/>
-      <c r="L95" s="13" t="s">
+      <c r="M95" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="M95" s="13"/>
-      <c r="N95" s="14" t="s">
+      <c r="N95" s="13"/>
+      <c r="O95" s="14" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H96" s="39"/>
       <c r="I96" s="32"/>
       <c r="J96" s="32"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N4" r:id="rId1" xr:uid="{AE0A5EED-E877-47F1-95C6-BFD4B992DCBE}"/>
-    <hyperlink ref="N5" r:id="rId2" xr:uid="{5AF98C2D-54A1-4433-A225-8EDA251E9782}"/>
-    <hyperlink ref="N6" r:id="rId3" xr:uid="{3BC9A1BA-B262-4227-8230-EFAFD41E9AE5}"/>
-    <hyperlink ref="N8" r:id="rId4" xr:uid="{1B3ECF74-0B44-4145-8ACA-5045787D820A}"/>
-    <hyperlink ref="N9" r:id="rId5" xr:uid="{38D8D2C0-99A0-43BE-B10C-8466CD0AEC0B}"/>
-    <hyperlink ref="N10" r:id="rId6" xr:uid="{24A4A094-2EC6-4AD2-9AC2-914048976E4A}"/>
-    <hyperlink ref="N11" r:id="rId7" xr:uid="{FAFECAD6-1904-44BB-BFE4-85ACEE9BFDE9}"/>
-    <hyperlink ref="N12" r:id="rId8" xr:uid="{C8852359-C5FE-4964-8FCE-9A90470981AA}"/>
-    <hyperlink ref="N7" r:id="rId9" xr:uid="{42CCD745-D6E9-4CB3-98ED-698D7775388D}"/>
-    <hyperlink ref="N17" r:id="rId10" xr:uid="{296994C2-7C61-4A7D-9F6F-3F68BD3D88C8}"/>
-    <hyperlink ref="N18" r:id="rId11" xr:uid="{366FBF39-E99D-4BD8-A888-68090C5AAB58}"/>
-    <hyperlink ref="N19" r:id="rId12" xr:uid="{C4D3AC60-B676-405A-999C-6D0BF36ADED4}"/>
-    <hyperlink ref="N21" r:id="rId13" xr:uid="{D056DB16-14E8-4139-BFBC-E689F4833646}"/>
-    <hyperlink ref="N22" r:id="rId14" xr:uid="{E9757565-0EC0-4CCA-8717-DD82F92D5BE5}"/>
-    <hyperlink ref="N23" r:id="rId15" xr:uid="{ECD78E6D-1DE0-4330-B8D5-B9C13121A6AB}"/>
-    <hyperlink ref="N24" r:id="rId16" xr:uid="{0E1136CC-BA1C-42C8-A639-D9B32A05E06C}"/>
-    <hyperlink ref="N25" r:id="rId17" xr:uid="{5CD4DE1A-1AEF-4258-B1CC-D4F89EBB2C6B}"/>
-    <hyperlink ref="N20" r:id="rId18" xr:uid="{85BD47E5-3027-424E-8EA5-63AFFCC79798}"/>
-    <hyperlink ref="N27" r:id="rId19" xr:uid="{429ECF84-3F17-453F-A8CD-FF5BB02F2C6E}"/>
-    <hyperlink ref="N29" r:id="rId20" xr:uid="{0FE4A098-5FFB-469E-B3D1-D7935DBDA769}"/>
-    <hyperlink ref="N34" r:id="rId21" xr:uid="{7666C554-894B-4540-90BF-A722F3355CC4}"/>
-    <hyperlink ref="N35" r:id="rId22" xr:uid="{69538AF5-D004-4BEB-97EC-EB9C44374090}"/>
-    <hyperlink ref="N36" r:id="rId23" xr:uid="{420F4813-1972-4E64-A982-ADA5E552B377}"/>
-    <hyperlink ref="N38" r:id="rId24" xr:uid="{EC86E1E1-6571-4A83-8A1D-A983BB036B1E}"/>
-    <hyperlink ref="N39" r:id="rId25" xr:uid="{16EBDAED-8A87-4584-B7D7-2887F94F81B1}"/>
-    <hyperlink ref="N40" r:id="rId26" xr:uid="{DD5A28AB-4507-4879-A577-695129FACBE0}"/>
-    <hyperlink ref="N41" r:id="rId27" xr:uid="{25CBFEB8-5CD6-4191-B7DF-DB3EF95DF242}"/>
-    <hyperlink ref="N37" r:id="rId28" xr:uid="{7C409F90-A335-4A77-9A97-A3BB765CE416}"/>
-    <hyperlink ref="O34" r:id="rId29" xr:uid="{F913FCC3-8AA8-4712-9550-63A79A632B66}"/>
-    <hyperlink ref="N46" r:id="rId30" xr:uid="{12401ABD-5BA9-40B9-8A98-F6E39B148C3B}"/>
-    <hyperlink ref="N47" r:id="rId31" xr:uid="{AF3A57FD-40EF-46EC-B641-DAEF2A50072A}"/>
-    <hyperlink ref="N48" r:id="rId32" xr:uid="{24792718-4D53-4BE7-ABC5-5E465087308B}"/>
-    <hyperlink ref="N50" r:id="rId33" xr:uid="{4D9FB32D-95E6-40B7-876E-CFA736652C2C}"/>
-    <hyperlink ref="N51" r:id="rId34" xr:uid="{6996CF09-5936-4A11-BCE6-4E07E56E161F}"/>
-    <hyperlink ref="N52" r:id="rId35" xr:uid="{2789BF76-D066-47BA-915F-41451578DF98}"/>
-    <hyperlink ref="N49" r:id="rId36" xr:uid="{568AD010-D627-4475-89F9-8F227E649F87}"/>
-    <hyperlink ref="N57" r:id="rId37" xr:uid="{0B7B1FE0-457A-4D24-8FFE-247BAADDEF1D}"/>
-    <hyperlink ref="N58" r:id="rId38" xr:uid="{47C5B8F0-CA12-4371-B567-F6CFFC886BB1}"/>
-    <hyperlink ref="N59" r:id="rId39" xr:uid="{153797E4-E21F-4DF1-A95A-1C1390B81B93}"/>
-    <hyperlink ref="N61" r:id="rId40" xr:uid="{53E48E75-7DF9-4FA3-8E37-AAC0E9E51728}"/>
-    <hyperlink ref="N62" r:id="rId41" xr:uid="{771E4588-E60D-41E5-9EB1-AB6780B56CB3}"/>
-    <hyperlink ref="N63" r:id="rId42" xr:uid="{313D817E-2E75-47AA-8E2B-EE178E69E72B}"/>
-    <hyperlink ref="N64" r:id="rId43" xr:uid="{9FCF0F96-85B5-4DB8-B3E8-6E5AAF72575B}"/>
-    <hyperlink ref="N65" r:id="rId44" xr:uid="{14274367-6B0C-4F46-8AF7-BE44A88610DA}"/>
-    <hyperlink ref="N60" r:id="rId45" xr:uid="{B060C748-0A75-43B2-8148-EA9539BEDA6C}"/>
-    <hyperlink ref="N67" r:id="rId46" xr:uid="{9337F166-DBED-4D36-BEFF-5F314FBC92C4}"/>
-    <hyperlink ref="N72" r:id="rId47" xr:uid="{D6A35461-8F4E-48A3-BCC2-8452A007F42F}"/>
-    <hyperlink ref="N74" r:id="rId48" xr:uid="{A1E15E18-865A-428D-BD73-4D7854A3F882}"/>
-    <hyperlink ref="N75" r:id="rId49" xr:uid="{FC4A0CF8-E5E5-4A69-A79A-BE581DE1B753}"/>
-    <hyperlink ref="N78" r:id="rId50" xr:uid="{FA1EEF9B-8870-4C99-ABA1-FFCDFC67258F}"/>
-    <hyperlink ref="N79" r:id="rId51" xr:uid="{6DF3237B-F457-48C8-9ACA-51051688FE23}"/>
-    <hyperlink ref="N80" r:id="rId52" xr:uid="{62C9B97A-2788-4F90-AA2A-579EC1BD7CEF}"/>
-    <hyperlink ref="N81" r:id="rId53" xr:uid="{B63B3740-BF73-4EB4-8635-B589531BBB36}"/>
-    <hyperlink ref="N76" r:id="rId54" xr:uid="{59C18176-78F0-4E26-8E5F-69C860CABC51}"/>
-    <hyperlink ref="N83" r:id="rId55" xr:uid="{7A459DA2-0FC2-4564-9A81-8B699BFD551F}"/>
-    <hyperlink ref="N82" r:id="rId56" xr:uid="{7B6C5D0A-9805-4C5D-8CCC-4049D2B4396F}"/>
-    <hyperlink ref="N84" r:id="rId57" xr:uid="{22AE91FC-178D-43F2-9391-FD91305E2C3A}"/>
-    <hyperlink ref="N85" r:id="rId58" xr:uid="{8AF0D46F-6402-495B-9DB4-95C4115C5BF3}"/>
-    <hyperlink ref="N73" r:id="rId59" xr:uid="{0589E4C5-E0F8-4D62-810B-5A2493891FA7}"/>
-    <hyperlink ref="N90" r:id="rId60" xr:uid="{D88FBCC2-E2E1-46EA-A873-4913F32E563D}"/>
-    <hyperlink ref="N91" r:id="rId61" xr:uid="{A877EDB9-FFDB-4C1E-9598-EE8A41A1DDE5}"/>
-    <hyperlink ref="N92" r:id="rId62" xr:uid="{97B73E21-A956-4577-85E7-3BFE1A5499DA}"/>
-    <hyperlink ref="N94" r:id="rId63" xr:uid="{21CD9E27-A5CE-4C8A-9537-B717BD2CACCC}"/>
-    <hyperlink ref="N95" r:id="rId64" xr:uid="{823665A7-821A-4643-AEDC-8AE4D6B1F8B7}"/>
-    <hyperlink ref="N93" r:id="rId65" xr:uid="{197354A2-B6D6-47E9-B520-B865F7918954}"/>
+    <hyperlink ref="O4" r:id="rId1" xr:uid="{AE0A5EED-E877-47F1-95C6-BFD4B992DCBE}"/>
+    <hyperlink ref="O5" r:id="rId2" xr:uid="{5AF98C2D-54A1-4433-A225-8EDA251E9782}"/>
+    <hyperlink ref="O6" r:id="rId3" xr:uid="{3BC9A1BA-B262-4227-8230-EFAFD41E9AE5}"/>
+    <hyperlink ref="O8" r:id="rId4" xr:uid="{1B3ECF74-0B44-4145-8ACA-5045787D820A}"/>
+    <hyperlink ref="O9" r:id="rId5" xr:uid="{38D8D2C0-99A0-43BE-B10C-8466CD0AEC0B}"/>
+    <hyperlink ref="O10" r:id="rId6" xr:uid="{24A4A094-2EC6-4AD2-9AC2-914048976E4A}"/>
+    <hyperlink ref="O11" r:id="rId7" xr:uid="{FAFECAD6-1904-44BB-BFE4-85ACEE9BFDE9}"/>
+    <hyperlink ref="O12" r:id="rId8" xr:uid="{C8852359-C5FE-4964-8FCE-9A90470981AA}"/>
+    <hyperlink ref="O7" r:id="rId9" xr:uid="{42CCD745-D6E9-4CB3-98ED-698D7775388D}"/>
+    <hyperlink ref="O17" r:id="rId10" xr:uid="{296994C2-7C61-4A7D-9F6F-3F68BD3D88C8}"/>
+    <hyperlink ref="O18" r:id="rId11" xr:uid="{366FBF39-E99D-4BD8-A888-68090C5AAB58}"/>
+    <hyperlink ref="O19" r:id="rId12" xr:uid="{C4D3AC60-B676-405A-999C-6D0BF36ADED4}"/>
+    <hyperlink ref="O21" r:id="rId13" xr:uid="{D056DB16-14E8-4139-BFBC-E689F4833646}"/>
+    <hyperlink ref="O22" r:id="rId14" xr:uid="{E9757565-0EC0-4CCA-8717-DD82F92D5BE5}"/>
+    <hyperlink ref="O23" r:id="rId15" xr:uid="{ECD78E6D-1DE0-4330-B8D5-B9C13121A6AB}"/>
+    <hyperlink ref="O24" r:id="rId16" xr:uid="{0E1136CC-BA1C-42C8-A639-D9B32A05E06C}"/>
+    <hyperlink ref="O25" r:id="rId17" xr:uid="{5CD4DE1A-1AEF-4258-B1CC-D4F89EBB2C6B}"/>
+    <hyperlink ref="O20" r:id="rId18" xr:uid="{85BD47E5-3027-424E-8EA5-63AFFCC79798}"/>
+    <hyperlink ref="O27" r:id="rId19" xr:uid="{429ECF84-3F17-453F-A8CD-FF5BB02F2C6E}"/>
+    <hyperlink ref="O29" r:id="rId20" xr:uid="{0FE4A098-5FFB-469E-B3D1-D7935DBDA769}"/>
+    <hyperlink ref="O34" r:id="rId21" xr:uid="{7666C554-894B-4540-90BF-A722F3355CC4}"/>
+    <hyperlink ref="O35" r:id="rId22" xr:uid="{69538AF5-D004-4BEB-97EC-EB9C44374090}"/>
+    <hyperlink ref="O36" r:id="rId23" xr:uid="{420F4813-1972-4E64-A982-ADA5E552B377}"/>
+    <hyperlink ref="O38" r:id="rId24" xr:uid="{EC86E1E1-6571-4A83-8A1D-A983BB036B1E}"/>
+    <hyperlink ref="O39" r:id="rId25" xr:uid="{16EBDAED-8A87-4584-B7D7-2887F94F81B1}"/>
+    <hyperlink ref="O40" r:id="rId26" xr:uid="{DD5A28AB-4507-4879-A577-695129FACBE0}"/>
+    <hyperlink ref="O41" r:id="rId27" xr:uid="{25CBFEB8-5CD6-4191-B7DF-DB3EF95DF242}"/>
+    <hyperlink ref="O37" r:id="rId28" xr:uid="{7C409F90-A335-4A77-9A97-A3BB765CE416}"/>
+    <hyperlink ref="P34" r:id="rId29" xr:uid="{F913FCC3-8AA8-4712-9550-63A79A632B66}"/>
+    <hyperlink ref="O46" r:id="rId30" xr:uid="{12401ABD-5BA9-40B9-8A98-F6E39B148C3B}"/>
+    <hyperlink ref="O47" r:id="rId31" xr:uid="{AF3A57FD-40EF-46EC-B641-DAEF2A50072A}"/>
+    <hyperlink ref="O48" r:id="rId32" xr:uid="{24792718-4D53-4BE7-ABC5-5E465087308B}"/>
+    <hyperlink ref="O50" r:id="rId33" xr:uid="{4D9FB32D-95E6-40B7-876E-CFA736652C2C}"/>
+    <hyperlink ref="O51" r:id="rId34" xr:uid="{6996CF09-5936-4A11-BCE6-4E07E56E161F}"/>
+    <hyperlink ref="O52" r:id="rId35" xr:uid="{2789BF76-D066-47BA-915F-41451578DF98}"/>
+    <hyperlink ref="O49" r:id="rId36" xr:uid="{568AD010-D627-4475-89F9-8F227E649F87}"/>
+    <hyperlink ref="O57" r:id="rId37" xr:uid="{0B7B1FE0-457A-4D24-8FFE-247BAADDEF1D}"/>
+    <hyperlink ref="O58" r:id="rId38" xr:uid="{47C5B8F0-CA12-4371-B567-F6CFFC886BB1}"/>
+    <hyperlink ref="O59" r:id="rId39" xr:uid="{153797E4-E21F-4DF1-A95A-1C1390B81B93}"/>
+    <hyperlink ref="O61" r:id="rId40" xr:uid="{53E48E75-7DF9-4FA3-8E37-AAC0E9E51728}"/>
+    <hyperlink ref="O62" r:id="rId41" xr:uid="{771E4588-E60D-41E5-9EB1-AB6780B56CB3}"/>
+    <hyperlink ref="O63" r:id="rId42" xr:uid="{313D817E-2E75-47AA-8E2B-EE178E69E72B}"/>
+    <hyperlink ref="O64" r:id="rId43" xr:uid="{9FCF0F96-85B5-4DB8-B3E8-6E5AAF72575B}"/>
+    <hyperlink ref="O65" r:id="rId44" xr:uid="{14274367-6B0C-4F46-8AF7-BE44A88610DA}"/>
+    <hyperlink ref="O60" r:id="rId45" xr:uid="{B060C748-0A75-43B2-8148-EA9539BEDA6C}"/>
+    <hyperlink ref="O67" r:id="rId46" xr:uid="{9337F166-DBED-4D36-BEFF-5F314FBC92C4}"/>
+    <hyperlink ref="O72" r:id="rId47" xr:uid="{D6A35461-8F4E-48A3-BCC2-8452A007F42F}"/>
+    <hyperlink ref="O74" r:id="rId48" xr:uid="{A1E15E18-865A-428D-BD73-4D7854A3F882}"/>
+    <hyperlink ref="O75" r:id="rId49" xr:uid="{FC4A0CF8-E5E5-4A69-A79A-BE581DE1B753}"/>
+    <hyperlink ref="O78" r:id="rId50" xr:uid="{FA1EEF9B-8870-4C99-ABA1-FFCDFC67258F}"/>
+    <hyperlink ref="O79" r:id="rId51" xr:uid="{6DF3237B-F457-48C8-9ACA-51051688FE23}"/>
+    <hyperlink ref="O80" r:id="rId52" xr:uid="{62C9B97A-2788-4F90-AA2A-579EC1BD7CEF}"/>
+    <hyperlink ref="O81" r:id="rId53" xr:uid="{B63B3740-BF73-4EB4-8635-B589531BBB36}"/>
+    <hyperlink ref="O76" r:id="rId54" xr:uid="{59C18176-78F0-4E26-8E5F-69C860CABC51}"/>
+    <hyperlink ref="O83" r:id="rId55" xr:uid="{7A459DA2-0FC2-4564-9A81-8B699BFD551F}"/>
+    <hyperlink ref="O82" r:id="rId56" xr:uid="{7B6C5D0A-9805-4C5D-8CCC-4049D2B4396F}"/>
+    <hyperlink ref="O84" r:id="rId57" xr:uid="{22AE91FC-178D-43F2-9391-FD91305E2C3A}"/>
+    <hyperlink ref="O85" r:id="rId58" xr:uid="{8AF0D46F-6402-495B-9DB4-95C4115C5BF3}"/>
+    <hyperlink ref="O73" r:id="rId59" xr:uid="{0589E4C5-E0F8-4D62-810B-5A2493891FA7}"/>
+    <hyperlink ref="O90" r:id="rId60" xr:uid="{D88FBCC2-E2E1-46EA-A873-4913F32E563D}"/>
+    <hyperlink ref="O91" r:id="rId61" xr:uid="{A877EDB9-FFDB-4C1E-9598-EE8A41A1DDE5}"/>
+    <hyperlink ref="O92" r:id="rId62" xr:uid="{97B73E21-A956-4577-85E7-3BFE1A5499DA}"/>
+    <hyperlink ref="O94" r:id="rId63" xr:uid="{21CD9E27-A5CE-4C8A-9537-B717BD2CACCC}"/>
+    <hyperlink ref="O95" r:id="rId64" xr:uid="{823665A7-821A-4643-AEDC-8AE4D6B1F8B7}"/>
+    <hyperlink ref="O93" r:id="rId65" xr:uid="{197354A2-B6D6-47E9-B520-B865F7918954}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId66"/>

</xml_diff>

<commit_message>
05_25 new files and task
</commit_message>
<xml_diff>
--- a/Gyerekek.xlsx
+++ b/Gyerekek.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Privat\Informatika\Github\ZitaTuroczi1.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E24F11F-1A6E-4238-B24D-AF6882899F6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5052DB41-F509-4819-8E22-42931FC25D5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15705" yWindow="795" windowWidth="12690" windowHeight="14880" xr2:uid="{D8DA68CD-37D4-4C3C-BD5C-8E37EBBBD311}"/>
+    <workbookView xWindow="13230" yWindow="795" windowWidth="12690" windowHeight="14880" xr2:uid="{D8DA68CD-37D4-4C3C-BD5C-8E37EBBBD311}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="230">
   <si>
     <t xml:space="preserve">Előképző 
 </t>
@@ -719,6 +719,9 @@
   </si>
   <si>
     <t>Mécsestartó</t>
+  </si>
+  <si>
+    <t>Vitorlás</t>
   </si>
 </sst>
 </file>
@@ -767,7 +770,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -978,12 +981,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
@@ -1062,6 +1074,13 @@
       <alignment textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hivatkozás" xfId="1" builtinId="8"/>
@@ -1379,8 +1398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9286C3FF-60BE-42C4-89D5-9ACF7C2ACF54}">
   <dimension ref="A2:P96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N36" sqref="N36"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M71" sqref="M71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1421,7 +1440,9 @@
       <c r="H2" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="I2" s="33"/>
+      <c r="I2" s="2" t="s">
+        <v>229</v>
+      </c>
       <c r="J2" s="33"/>
     </row>
     <row r="3" spans="1:15" s="1" customFormat="1" ht="42" thickBot="1" x14ac:dyDescent="0.3">
@@ -1447,7 +1468,9 @@
       <c r="H3" s="8">
         <v>43950</v>
       </c>
-      <c r="I3" s="34"/>
+      <c r="I3" s="8">
+        <v>43977</v>
+      </c>
       <c r="J3" s="34"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -1463,7 +1486,7 @@
       <c r="F4" s="23"/>
       <c r="G4" s="20"/>
       <c r="H4" s="20"/>
-      <c r="I4" s="32"/>
+      <c r="I4" s="20"/>
       <c r="J4" s="32"/>
       <c r="M4" s="13" t="s">
         <v>11</v>
@@ -1486,7 +1509,7 @@
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
       <c r="H5" s="22"/>
-      <c r="I5" s="32"/>
+      <c r="I5" s="15"/>
       <c r="J5" s="32"/>
       <c r="M5" s="13" t="s">
         <v>13</v>
@@ -1511,7 +1534,7 @@
       <c r="F6" s="22"/>
       <c r="G6" s="22"/>
       <c r="H6" s="22"/>
-      <c r="I6" s="32"/>
+      <c r="I6" s="15"/>
       <c r="J6" s="32"/>
       <c r="M6" s="13" t="s">
         <v>16</v>
@@ -1536,7 +1559,7 @@
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
-      <c r="I7" s="32"/>
+      <c r="I7" s="15"/>
       <c r="J7" s="32"/>
       <c r="M7" s="13" t="s">
         <v>20</v>
@@ -1559,7 +1582,7 @@
       <c r="F8" s="22"/>
       <c r="G8" s="22"/>
       <c r="H8" s="15"/>
-      <c r="I8" s="32"/>
+      <c r="I8" s="15"/>
       <c r="J8" s="32"/>
       <c r="M8" s="13" t="s">
         <v>22</v>
@@ -1582,7 +1605,7 @@
       <c r="F9" s="22"/>
       <c r="G9" s="22"/>
       <c r="H9" s="22"/>
-      <c r="I9" s="32"/>
+      <c r="I9" s="15"/>
       <c r="J9" s="32"/>
       <c r="M9" s="13" t="s">
         <v>23</v>
@@ -1607,7 +1630,7 @@
       <c r="F10" s="22"/>
       <c r="G10" s="22"/>
       <c r="H10" s="22"/>
-      <c r="I10" s="32"/>
+      <c r="I10" s="15"/>
       <c r="J10" s="32"/>
       <c r="M10" s="13" t="s">
         <v>26</v>
@@ -1632,7 +1655,7 @@
       <c r="F11" s="22"/>
       <c r="G11" s="22"/>
       <c r="H11" s="22"/>
-      <c r="I11" s="32"/>
+      <c r="I11" s="15"/>
       <c r="J11" s="32"/>
       <c r="M11" s="13" t="s">
         <v>29</v>
@@ -1655,7 +1678,7 @@
       <c r="F12" s="22"/>
       <c r="G12" s="22"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="32"/>
+      <c r="I12" s="15"/>
       <c r="J12" s="32"/>
       <c r="M12" s="13" t="s">
         <v>32</v>
@@ -1692,7 +1715,9 @@
       <c r="H15" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="I15" s="33"/>
+      <c r="I15" s="2" t="s">
+        <v>229</v>
+      </c>
       <c r="J15" s="33"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -1723,7 +1748,9 @@
       <c r="H16" s="8">
         <v>43950</v>
       </c>
-      <c r="I16" s="34"/>
+      <c r="I16" s="8">
+        <v>43977</v>
+      </c>
       <c r="J16" s="34"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -1744,7 +1771,7 @@
       <c r="F17" s="23"/>
       <c r="G17" s="23"/>
       <c r="H17" s="20"/>
-      <c r="I17" s="32"/>
+      <c r="I17" s="20"/>
       <c r="J17" s="32"/>
       <c r="M17" s="13" t="s">
         <v>48</v>
@@ -1767,7 +1794,7 @@
       <c r="F18" s="22"/>
       <c r="G18" s="22"/>
       <c r="H18" s="22"/>
-      <c r="I18" s="32"/>
+      <c r="I18" s="15"/>
       <c r="J18" s="32"/>
       <c r="M18" s="13" t="s">
         <v>50</v>
@@ -1792,7 +1819,7 @@
       <c r="F19" s="22"/>
       <c r="G19" s="22"/>
       <c r="H19" s="22"/>
-      <c r="I19" s="32"/>
+      <c r="I19" s="15"/>
       <c r="J19" s="32"/>
       <c r="M19" s="13" t="s">
         <v>53</v>
@@ -1817,7 +1844,7 @@
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
-      <c r="I20" s="32"/>
+      <c r="I20" s="15"/>
       <c r="J20" s="32"/>
       <c r="M20" s="13" t="s">
         <v>56</v>
@@ -1840,7 +1867,7 @@
       <c r="F21" s="22"/>
       <c r="G21" s="22"/>
       <c r="H21" s="22"/>
-      <c r="I21" s="32"/>
+      <c r="I21" s="15"/>
       <c r="J21" s="32"/>
       <c r="M21" s="13" t="s">
         <v>58</v>
@@ -1862,8 +1889,8 @@
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
       <c r="G22" s="22"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="32"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="15"/>
       <c r="J22" s="32"/>
       <c r="M22" s="13" t="s">
         <v>60</v>
@@ -1886,7 +1913,7 @@
       <c r="F23" s="22"/>
       <c r="G23" s="22"/>
       <c r="H23" s="15"/>
-      <c r="I23" s="32"/>
+      <c r="I23" s="15"/>
       <c r="J23" s="32"/>
       <c r="M23" s="13" t="s">
         <v>62</v>
@@ -1909,7 +1936,7 @@
       <c r="F24" s="22"/>
       <c r="G24" s="22"/>
       <c r="H24" s="22"/>
-      <c r="I24" s="32"/>
+      <c r="I24" s="15"/>
       <c r="J24" s="32"/>
       <c r="M24" s="13" t="s">
         <v>64</v>
@@ -1932,7 +1959,7 @@
       <c r="F25" s="22"/>
       <c r="G25" s="22"/>
       <c r="H25" s="22"/>
-      <c r="I25" s="32"/>
+      <c r="I25" s="15"/>
       <c r="J25" s="32"/>
       <c r="M25" s="13" t="s">
         <v>66</v>
@@ -1955,7 +1982,7 @@
       <c r="F26" s="22"/>
       <c r="G26" s="22"/>
       <c r="H26" s="22"/>
-      <c r="I26" s="32"/>
+      <c r="I26" s="15"/>
       <c r="J26" s="32"/>
       <c r="M26" s="13" t="s">
         <v>68</v>
@@ -1976,7 +2003,7 @@
       <c r="F27" s="22"/>
       <c r="G27" s="3"/>
       <c r="H27" s="22"/>
-      <c r="I27" s="32"/>
+      <c r="I27" s="15"/>
       <c r="J27" s="32"/>
       <c r="M27" s="13" t="s">
         <v>69</v>
@@ -2001,7 +2028,7 @@
       <c r="F28" s="22"/>
       <c r="G28" s="3"/>
       <c r="H28" s="22"/>
-      <c r="I28" s="32"/>
+      <c r="I28" s="15"/>
       <c r="J28" s="32"/>
       <c r="M28" s="13"/>
       <c r="N28" s="13"/>
@@ -2020,7 +2047,7 @@
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
       <c r="H29" s="3"/>
-      <c r="I29" s="32"/>
+      <c r="I29" s="15"/>
       <c r="J29" s="32"/>
       <c r="M29" s="13" t="s">
         <v>71</v>
@@ -2055,7 +2082,9 @@
       <c r="H32" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="I32" s="33"/>
+      <c r="I32" s="2" t="s">
+        <v>229</v>
+      </c>
       <c r="J32" s="33"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
@@ -2086,7 +2115,9 @@
       <c r="H33" s="8">
         <v>43950</v>
       </c>
-      <c r="I33" s="34"/>
+      <c r="I33" s="8">
+        <v>43977</v>
+      </c>
       <c r="J33" s="34"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
@@ -2107,7 +2138,7 @@
       <c r="F34" s="23"/>
       <c r="G34" s="20"/>
       <c r="H34" s="23"/>
-      <c r="I34" s="32"/>
+      <c r="I34" s="20"/>
       <c r="J34" s="32"/>
       <c r="M34" s="13" t="s">
         <v>81</v>
@@ -2135,7 +2166,7 @@
       <c r="F35" s="22"/>
       <c r="G35" s="22"/>
       <c r="H35" s="22"/>
-      <c r="I35" s="32"/>
+      <c r="I35" s="15"/>
       <c r="J35" s="32"/>
       <c r="M35" s="13" t="s">
         <v>85</v>
@@ -2158,7 +2189,7 @@
       <c r="F36" s="22"/>
       <c r="G36" s="22"/>
       <c r="H36" s="22"/>
-      <c r="I36" s="32"/>
+      <c r="I36" s="15"/>
       <c r="J36" s="32"/>
       <c r="M36" s="13" t="s">
         <v>87</v>
@@ -2181,7 +2212,7 @@
       <c r="F37" s="22"/>
       <c r="G37" s="22"/>
       <c r="H37" s="22"/>
-      <c r="I37" s="32"/>
+      <c r="I37" s="15"/>
       <c r="J37" s="32"/>
       <c r="M37" s="13" t="s">
         <v>88</v>
@@ -2204,7 +2235,7 @@
       <c r="F38" s="22"/>
       <c r="G38" s="22"/>
       <c r="H38" s="15"/>
-      <c r="I38" s="32"/>
+      <c r="I38" s="15"/>
       <c r="J38" s="32"/>
       <c r="M38" s="13" t="s">
         <v>90</v>
@@ -2227,7 +2258,7 @@
       <c r="F39" s="22"/>
       <c r="G39" s="22"/>
       <c r="H39" s="22"/>
-      <c r="I39" s="32"/>
+      <c r="I39" s="15"/>
       <c r="J39" s="32"/>
       <c r="M39" s="13" t="s">
         <v>92</v>
@@ -2250,7 +2281,7 @@
       <c r="F40" s="22"/>
       <c r="G40" s="15"/>
       <c r="H40" s="15"/>
-      <c r="I40" s="32"/>
+      <c r="I40" s="15"/>
       <c r="J40" s="32"/>
       <c r="M40" s="13" t="s">
         <v>94</v>
@@ -2275,7 +2306,7 @@
       <c r="F41" s="22"/>
       <c r="G41" s="22"/>
       <c r="H41" s="22"/>
-      <c r="I41" s="32"/>
+      <c r="I41" s="15"/>
       <c r="J41" s="32"/>
       <c r="M41" s="13" t="s">
         <v>97</v>
@@ -2314,9 +2345,6 @@
         <v>223</v>
       </c>
       <c r="J44" s="35" t="s">
-        <v>226</v>
-      </c>
-      <c r="K44" s="35" t="s">
         <v>228</v>
       </c>
       <c r="L44" s="1"/>
@@ -2351,9 +2379,6 @@
         <v>43958</v>
       </c>
       <c r="J45" s="36">
-        <v>43965</v>
-      </c>
-      <c r="K45" s="36">
         <v>43972</v>
       </c>
       <c r="L45" s="1"/>
@@ -2376,7 +2401,6 @@
       <c r="H46" s="20"/>
       <c r="I46" s="20"/>
       <c r="J46" s="20"/>
-      <c r="K46" s="20"/>
       <c r="M46" s="13" t="s">
         <v>107</v>
       </c>
@@ -2400,7 +2424,6 @@
       <c r="H47" s="15"/>
       <c r="I47" s="15"/>
       <c r="J47" s="15"/>
-      <c r="K47" s="15"/>
       <c r="M47" s="13" t="s">
         <v>109</v>
       </c>
@@ -2424,7 +2447,6 @@
       <c r="H48" s="22"/>
       <c r="I48" s="15"/>
       <c r="J48" s="15"/>
-      <c r="K48" s="15"/>
       <c r="M48" s="13" t="s">
         <v>111</v>
       </c>
@@ -2450,7 +2472,6 @@
       <c r="H49" s="22"/>
       <c r="I49" s="22"/>
       <c r="J49" s="15"/>
-      <c r="K49" s="15"/>
       <c r="M49" s="13" t="s">
         <v>115</v>
       </c>
@@ -2474,7 +2495,6 @@
       <c r="H50" s="15"/>
       <c r="I50" s="22"/>
       <c r="J50" s="15"/>
-      <c r="K50" s="15"/>
       <c r="M50" s="13" t="s">
         <v>116</v>
       </c>
@@ -2498,7 +2518,6 @@
       <c r="H51" s="22"/>
       <c r="I51" s="15"/>
       <c r="J51" s="15"/>
-      <c r="K51" s="15"/>
       <c r="M51" s="13" t="s">
         <v>118</v>
       </c>
@@ -2522,7 +2541,6 @@
       <c r="H52" s="22"/>
       <c r="I52" s="22"/>
       <c r="J52" s="15"/>
-      <c r="K52" s="15"/>
       <c r="M52" s="13" t="s">
         <v>120</v>
       </c>
@@ -2902,9 +2920,7 @@
       <c r="J70" s="35" t="s">
         <v>226</v>
       </c>
-      <c r="K70" s="35" t="s">
-        <v>228</v>
-      </c>
+      <c r="K70" s="40"/>
       <c r="L70" s="1"/>
       <c r="M70" s="1"/>
       <c r="N70" s="1"/>
@@ -2939,9 +2955,7 @@
       <c r="J71" s="36">
         <v>43965</v>
       </c>
-      <c r="K71" s="36">
-        <v>43972</v>
-      </c>
+      <c r="K71" s="41"/>
       <c r="L71" s="1"/>
       <c r="M71" s="1"/>
       <c r="N71" s="1"/>
@@ -2962,7 +2976,7 @@
       <c r="H72" s="4"/>
       <c r="I72" s="23"/>
       <c r="J72" s="20"/>
-      <c r="K72" s="20"/>
+      <c r="K72" s="42"/>
       <c r="M72" s="13" t="s">
         <v>168</v>
       </c>
@@ -2988,7 +3002,7 @@
       <c r="H73" s="22"/>
       <c r="I73" s="22"/>
       <c r="J73" s="22"/>
-      <c r="K73" s="15"/>
+      <c r="K73" s="42"/>
       <c r="M73" s="13" t="s">
         <v>48</v>
       </c>
@@ -3011,7 +3025,7 @@
       <c r="H74" s="3"/>
       <c r="I74" s="15"/>
       <c r="J74" s="15"/>
-      <c r="K74" s="15"/>
+      <c r="K74" s="42"/>
       <c r="M74" s="13" t="s">
         <v>171</v>
       </c>
@@ -3035,7 +3049,7 @@
       <c r="H75" s="22"/>
       <c r="I75" s="22"/>
       <c r="J75" s="15"/>
-      <c r="K75" s="15"/>
+      <c r="K75" s="42"/>
       <c r="M75" s="13" t="s">
         <v>173</v>
       </c>
@@ -3059,7 +3073,7 @@
       <c r="H76" s="22"/>
       <c r="I76" s="22"/>
       <c r="J76" s="15"/>
-      <c r="K76" s="15"/>
+      <c r="K76" s="42"/>
       <c r="M76" s="13" t="s">
         <v>85</v>
       </c>
@@ -3083,7 +3097,7 @@
       <c r="H77" s="3"/>
       <c r="I77" s="15"/>
       <c r="J77" s="15"/>
-      <c r="K77" s="15"/>
+      <c r="K77" s="42"/>
       <c r="M77" s="13"/>
       <c r="N77" s="13"/>
       <c r="O77" s="14"/>
@@ -3103,7 +3117,7 @@
       <c r="H78" s="22"/>
       <c r="I78" s="22"/>
       <c r="J78" s="22"/>
-      <c r="K78" s="15"/>
+      <c r="K78" s="42"/>
       <c r="M78" s="13" t="s">
         <v>87</v>
       </c>
@@ -3127,7 +3141,7 @@
       <c r="H79" s="22"/>
       <c r="I79" s="22"/>
       <c r="J79" s="15"/>
-      <c r="K79" s="15"/>
+      <c r="K79" s="42"/>
       <c r="M79" s="13" t="s">
         <v>176</v>
       </c>
@@ -3151,7 +3165,7 @@
       <c r="H80" s="22"/>
       <c r="I80" s="22"/>
       <c r="J80" s="15"/>
-      <c r="K80" s="15"/>
+      <c r="K80" s="42"/>
       <c r="M80" s="13" t="s">
         <v>178</v>
       </c>
@@ -3175,7 +3189,7 @@
       <c r="H81" s="22"/>
       <c r="I81" s="22"/>
       <c r="J81" s="15"/>
-      <c r="K81" s="15"/>
+      <c r="K81" s="42"/>
       <c r="M81" s="13" t="s">
         <v>180</v>
       </c>
@@ -3199,7 +3213,7 @@
       <c r="H82" s="3"/>
       <c r="I82" s="22"/>
       <c r="J82" s="15"/>
-      <c r="K82" s="15"/>
+      <c r="K82" s="42"/>
       <c r="M82" s="13" t="s">
         <v>182</v>
       </c>
@@ -3223,7 +3237,7 @@
       <c r="H83" s="3"/>
       <c r="I83" s="15"/>
       <c r="J83" s="15"/>
-      <c r="K83" s="15"/>
+      <c r="K83" s="42"/>
       <c r="M83" s="13" t="s">
         <v>184</v>
       </c>
@@ -3247,7 +3261,7 @@
       <c r="H84" s="22"/>
       <c r="I84" s="22"/>
       <c r="J84" s="15"/>
-      <c r="K84" s="15"/>
+      <c r="K84" s="42"/>
       <c r="M84" s="13" t="s">
         <v>186</v>
       </c>
@@ -3273,7 +3287,7 @@
       <c r="H85" s="22"/>
       <c r="I85" s="22"/>
       <c r="J85" s="15"/>
-      <c r="K85" s="15"/>
+      <c r="K85" s="42"/>
       <c r="M85" s="13" t="s">
         <v>187</v>
       </c>

</xml_diff>